<commit_message>
minor update in plug width spreadsheet
</commit_message>
<xml_diff>
--- a/data/PlugWidthEvaluation.xlsx
+++ b/data/PlugWidthEvaluation.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brghena\Dropbox\repos\powerblade\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -973,6 +968,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -982,37 +993,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1531,11 +1526,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="345737504"/>
-        <c:axId val="345741424"/>
+        <c:axId val="74446336"/>
+        <c:axId val="74448256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="345737504"/>
+        <c:axId val="74446336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1564,7 +1559,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="345741424"/>
+        <c:crossAx val="74448256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1572,7 +1567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="345741424"/>
+        <c:axId val="74448256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1601,7 +1596,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="345737504"/>
+        <c:crossAx val="74446336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1701,7 +1696,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1736,7 +1731,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1947,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O166"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,14 +1959,14 @@
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="J2" s="41" t="s">
+      <c r="F2" s="52"/>
+      <c r="J2" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="42"/>
+      <c r="K2" s="52"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -2069,19 +2064,19 @@
         <v>165</v>
       </c>
       <c r="C7" s="32">
-        <v>0.36599999999999999</v>
+        <v>0.36499999999999999</v>
       </c>
       <c r="D7" s="15">
         <f>C7-0.29</f>
-        <v>7.6000000000000012E-2</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="E7" s="8">
         <f t="shared" si="0"/>
-        <v>0.53600000000000003</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" si="1"/>
-        <v>0.57999999999999996</v>
+        <v>0.57799999999999996</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2298,11 +2293,11 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5">
         <f>COUNTIF(Data!R19:R1000,"Y")</f>
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M19" s="37">
         <f>COUNTIF(Data!R19:R1000,"N")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
@@ -2321,11 +2316,11 @@
       <c r="K20" s="39"/>
       <c r="L20" s="39">
         <f>COUNTIF(Data!U19:U1000,"Good")</f>
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M20" s="40">
         <f>L9-L20</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
@@ -3164,7 +3159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A17:AM176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="16" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="Z10" sqref="Z10"/>
@@ -3197,57 +3192,57 @@
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
-      <c r="H17" s="45" t="s">
+      <c r="H17" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
       <c r="K17" s="19"/>
-      <c r="L17" s="45" t="s">
+      <c r="L17" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54"/>
       <c r="O17" s="19"/>
-      <c r="P17" s="45" t="s">
+      <c r="P17" s="54" t="s">
         <v>155</v>
       </c>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45" t="s">
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="54" t="s">
         <v>156</v>
       </c>
-      <c r="T17" s="45"/>
-      <c r="U17" s="45"/>
+      <c r="T17" s="54"/>
+      <c r="U17" s="54"/>
       <c r="V17" s="13"/>
-      <c r="W17" s="45" t="s">
+      <c r="W17" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="X17" s="45"/>
+      <c r="X17" s="54"/>
       <c r="Y17" s="13"/>
-      <c r="Z17" s="45" t="s">
+      <c r="Z17" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="AA17" s="45"/>
-      <c r="AC17" s="46" t="s">
+      <c r="AA17" s="54"/>
+      <c r="AC17" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="AD17" s="46"/>
-      <c r="AF17" s="44" t="s">
+      <c r="AD17" s="55"/>
+      <c r="AF17" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="AG17" s="44"/>
-      <c r="AI17" s="52" t="s">
+      <c r="AG17" s="58"/>
+      <c r="AI17" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="AJ17" s="52"/>
-      <c r="AK17" s="51" t="s">
+      <c r="AJ17" s="56"/>
+      <c r="AK17" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="AL17" s="53" t="s">
+      <c r="AL17" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="AM17" s="53"/>
+      <c r="AM17" s="57"/>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
@@ -3330,17 +3325,17 @@
       <c r="AG18" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="AI18" s="54" t="s">
+      <c r="AI18" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AJ18" s="54" t="s">
+      <c r="AJ18" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="AK18" s="55"/>
-      <c r="AL18" s="54" t="s">
+      <c r="AK18" s="47"/>
+      <c r="AL18" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AM18" s="54" t="s">
+      <c r="AM18" s="46" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3401,31 +3396,31 @@
         <f t="shared" ref="AA19:AA53" si="1">1000*(X19-0.29)</f>
         <v>64</v>
       </c>
-      <c r="AC19" s="49" t="s">
+      <c r="AC19" s="43" t="s">
         <v>203</v>
       </c>
       <c r="AD19" s="11">
         <f>COUNTIF($N$19:$N$165, "&lt;0.41")</f>
         <v>0</v>
       </c>
-      <c r="AF19" s="49" t="s">
+      <c r="AF19" s="43" t="s">
         <v>203</v>
       </c>
-      <c r="AG19" s="50">
+      <c r="AG19" s="44">
         <f>COUNTIF($J$19:$J$165, "&lt;0.41")</f>
         <v>0</v>
       </c>
-      <c r="AI19" s="56">
+      <c r="AI19" s="48">
         <v>0.41</v>
       </c>
-      <c r="AJ19" s="57">
+      <c r="AJ19" s="49">
         <v>0</v>
       </c>
-      <c r="AK19" s="55"/>
-      <c r="AL19" s="56">
+      <c r="AK19" s="47"/>
+      <c r="AL19" s="48">
         <v>0.41</v>
       </c>
-      <c r="AM19" s="57">
+      <c r="AM19" s="49">
         <v>0</v>
       </c>
     </row>
@@ -3500,17 +3495,17 @@
         <f>COUNTIF($J$19:$J$165, "&gt;="&amp;$AC20)-COUNTIF($J$19:$J$165,"&gt;="&amp;$AC21)</f>
         <v>0</v>
       </c>
-      <c r="AI20" s="56">
+      <c r="AI20" s="48">
         <v>0.41499999999999998</v>
       </c>
-      <c r="AJ20" s="57">
+      <c r="AJ20" s="49">
         <v>1</v>
       </c>
-      <c r="AK20" s="55"/>
-      <c r="AL20" s="56">
+      <c r="AK20" s="47"/>
+      <c r="AL20" s="48">
         <v>0.41499999999999998</v>
       </c>
-      <c r="AM20" s="57">
+      <c r="AM20" s="49">
         <v>0</v>
       </c>
     </row>
@@ -3585,17 +3580,17 @@
         <f t="shared" ref="AG21:AG50" si="3">COUNTIF($J$19:$J$165, "&gt;="&amp;$AC21)-COUNTIF($J$19:$J$165,"&gt;="&amp;$AC22)</f>
         <v>0</v>
       </c>
-      <c r="AI21" s="56">
+      <c r="AI21" s="48">
         <v>0.42</v>
       </c>
-      <c r="AJ21" s="57">
+      <c r="AJ21" s="49">
         <v>0</v>
       </c>
-      <c r="AK21" s="55"/>
-      <c r="AL21" s="56">
+      <c r="AK21" s="47"/>
+      <c r="AL21" s="48">
         <v>0.42</v>
       </c>
-      <c r="AM21" s="57">
+      <c r="AM21" s="49">
         <v>0</v>
       </c>
     </row>
@@ -3670,17 +3665,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI22" s="56">
+      <c r="AI22" s="48">
         <v>0.42499999999999999</v>
       </c>
-      <c r="AJ22" s="57">
+      <c r="AJ22" s="49">
         <v>1</v>
       </c>
-      <c r="AK22" s="55"/>
-      <c r="AL22" s="56">
+      <c r="AK22" s="47"/>
+      <c r="AL22" s="48">
         <v>0.42499999999999999</v>
       </c>
-      <c r="AM22" s="57">
+      <c r="AM22" s="49">
         <v>0</v>
       </c>
     </row>
@@ -3755,17 +3750,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI23" s="56">
+      <c r="AI23" s="48">
         <v>0.43</v>
       </c>
-      <c r="AJ23" s="57">
+      <c r="AJ23" s="49">
         <v>9</v>
       </c>
-      <c r="AK23" s="55"/>
-      <c r="AL23" s="56">
+      <c r="AK23" s="47"/>
+      <c r="AL23" s="48">
         <v>0.43</v>
       </c>
-      <c r="AM23" s="57">
+      <c r="AM23" s="49">
         <v>0</v>
       </c>
     </row>
@@ -3840,17 +3835,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI24" s="56">
+      <c r="AI24" s="48">
         <v>0.435</v>
       </c>
-      <c r="AJ24" s="57">
+      <c r="AJ24" s="49">
         <v>10</v>
       </c>
-      <c r="AK24" s="55"/>
-      <c r="AL24" s="56">
+      <c r="AK24" s="47"/>
+      <c r="AL24" s="48">
         <v>0.435</v>
       </c>
-      <c r="AM24" s="57">
+      <c r="AM24" s="49">
         <v>0</v>
       </c>
     </row>
@@ -3925,17 +3920,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI25" s="56">
+      <c r="AI25" s="48">
         <v>0.44</v>
       </c>
-      <c r="AJ25" s="57">
+      <c r="AJ25" s="49">
         <v>30</v>
       </c>
-      <c r="AK25" s="55"/>
-      <c r="AL25" s="56">
+      <c r="AK25" s="47"/>
+      <c r="AL25" s="48">
         <v>0.44</v>
       </c>
-      <c r="AM25" s="57">
+      <c r="AM25" s="49">
         <v>0</v>
       </c>
     </row>
@@ -4010,17 +4005,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI26" s="56">
+      <c r="AI26" s="48">
         <v>0.44500000000000001</v>
       </c>
-      <c r="AJ26" s="57">
+      <c r="AJ26" s="49">
         <v>20</v>
       </c>
-      <c r="AK26" s="55"/>
-      <c r="AL26" s="56">
+      <c r="AK26" s="47"/>
+      <c r="AL26" s="48">
         <v>0.44500000000000001</v>
       </c>
-      <c r="AM26" s="57">
+      <c r="AM26" s="49">
         <v>0</v>
       </c>
     </row>
@@ -4095,17 +4090,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI27" s="56">
+      <c r="AI27" s="48">
         <v>0.45</v>
       </c>
-      <c r="AJ27" s="57">
+      <c r="AJ27" s="49">
         <v>5</v>
       </c>
-      <c r="AK27" s="55"/>
-      <c r="AL27" s="56">
+      <c r="AK27" s="47"/>
+      <c r="AL27" s="48">
         <v>0.45</v>
       </c>
-      <c r="AM27" s="57">
+      <c r="AM27" s="49">
         <v>0</v>
       </c>
     </row>
@@ -4180,17 +4175,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI28" s="56">
+      <c r="AI28" s="48">
         <v>0.45500000000000002</v>
       </c>
-      <c r="AJ28" s="57">
+      <c r="AJ28" s="49">
         <v>1</v>
       </c>
-      <c r="AK28" s="55"/>
-      <c r="AL28" s="56">
+      <c r="AK28" s="47"/>
+      <c r="AL28" s="48">
         <v>0.45500000000000002</v>
       </c>
-      <c r="AM28" s="57">
+      <c r="AM28" s="49">
         <v>0</v>
       </c>
     </row>
@@ -4265,17 +4260,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI29" s="56">
+      <c r="AI29" s="48">
         <v>0.46</v>
       </c>
-      <c r="AJ29" s="57">
+      <c r="AJ29" s="49">
         <v>0</v>
       </c>
-      <c r="AK29" s="55"/>
-      <c r="AL29" s="56">
+      <c r="AK29" s="47"/>
+      <c r="AL29" s="48">
         <v>0.46</v>
       </c>
-      <c r="AM29" s="57">
+      <c r="AM29" s="49">
         <v>0</v>
       </c>
     </row>
@@ -4350,17 +4345,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI30" s="56">
+      <c r="AI30" s="48">
         <v>0.46500000000000002</v>
       </c>
-      <c r="AJ30" s="57">
+      <c r="AJ30" s="49">
         <v>0</v>
       </c>
-      <c r="AK30" s="55"/>
-      <c r="AL30" s="56">
+      <c r="AK30" s="47"/>
+      <c r="AL30" s="48">
         <v>0.46500000000000002</v>
       </c>
-      <c r="AM30" s="57">
+      <c r="AM30" s="49">
         <v>0</v>
       </c>
     </row>
@@ -4435,17 +4430,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI31" s="56">
+      <c r="AI31" s="48">
         <v>0.47</v>
       </c>
-      <c r="AJ31" s="57">
+      <c r="AJ31" s="49">
         <v>0</v>
       </c>
-      <c r="AK31" s="55"/>
-      <c r="AL31" s="56">
+      <c r="AK31" s="47"/>
+      <c r="AL31" s="48">
         <v>0.47</v>
       </c>
-      <c r="AM31" s="57">
+      <c r="AM31" s="49">
         <v>0</v>
       </c>
     </row>
@@ -4520,17 +4515,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI32" s="56">
+      <c r="AI32" s="48">
         <v>0.47499999999999998</v>
       </c>
-      <c r="AJ32" s="57">
+      <c r="AJ32" s="49">
         <v>0</v>
       </c>
-      <c r="AK32" s="55"/>
-      <c r="AL32" s="56">
+      <c r="AK32" s="47"/>
+      <c r="AL32" s="48">
         <v>0.47499999999999998</v>
       </c>
-      <c r="AM32" s="57">
+      <c r="AM32" s="49">
         <v>0</v>
       </c>
     </row>
@@ -4605,17 +4600,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI33" s="56">
+      <c r="AI33" s="48">
         <v>0.48</v>
       </c>
-      <c r="AJ33" s="57">
+      <c r="AJ33" s="49">
         <v>0</v>
       </c>
-      <c r="AK33" s="55"/>
-      <c r="AL33" s="56">
+      <c r="AK33" s="47"/>
+      <c r="AL33" s="48">
         <v>0.48</v>
       </c>
-      <c r="AM33" s="57">
+      <c r="AM33" s="49">
         <v>0</v>
       </c>
     </row>
@@ -4690,17 +4685,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI34" s="56">
+      <c r="AI34" s="48">
         <v>0.48499999999999999</v>
       </c>
-      <c r="AJ34" s="57">
+      <c r="AJ34" s="49">
         <v>0</v>
       </c>
-      <c r="AK34" s="55"/>
-      <c r="AL34" s="56">
+      <c r="AK34" s="47"/>
+      <c r="AL34" s="48">
         <v>0.48499999999999999</v>
       </c>
-      <c r="AM34" s="57">
+      <c r="AM34" s="49">
         <v>0</v>
       </c>
     </row>
@@ -4775,17 +4770,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI35" s="56">
+      <c r="AI35" s="48">
         <v>0.51</v>
       </c>
-      <c r="AJ35" s="57">
+      <c r="AJ35" s="49">
         <v>0</v>
       </c>
-      <c r="AK35" s="55"/>
-      <c r="AL35" s="56">
+      <c r="AK35" s="47"/>
+      <c r="AL35" s="48">
         <v>0.51</v>
       </c>
-      <c r="AM35" s="57">
+      <c r="AM35" s="49">
         <v>0</v>
       </c>
     </row>
@@ -4860,17 +4855,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI36" s="56">
+      <c r="AI36" s="48">
         <v>0.51500000000000001</v>
       </c>
-      <c r="AJ36" s="57">
+      <c r="AJ36" s="49">
         <v>0</v>
       </c>
-      <c r="AK36" s="55"/>
-      <c r="AL36" s="56">
+      <c r="AK36" s="47"/>
+      <c r="AL36" s="48">
         <v>0.51500000000000001</v>
       </c>
-      <c r="AM36" s="57">
+      <c r="AM36" s="49">
         <v>0</v>
       </c>
     </row>
@@ -4945,17 +4940,17 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AI37" s="56">
+      <c r="AI37" s="48">
         <v>0.52</v>
       </c>
-      <c r="AJ37" s="57">
+      <c r="AJ37" s="49">
         <v>0</v>
       </c>
-      <c r="AK37" s="55"/>
-      <c r="AL37" s="56">
+      <c r="AK37" s="47"/>
+      <c r="AL37" s="48">
         <v>0.52</v>
       </c>
-      <c r="AM37" s="57">
+      <c r="AM37" s="49">
         <v>1</v>
       </c>
     </row>
@@ -5030,17 +5025,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI38" s="56">
+      <c r="AI38" s="48">
         <v>0.52500000000000002</v>
       </c>
-      <c r="AJ38" s="57">
+      <c r="AJ38" s="49">
         <v>0</v>
       </c>
-      <c r="AK38" s="55"/>
-      <c r="AL38" s="56">
+      <c r="AK38" s="47"/>
+      <c r="AL38" s="48">
         <v>0.52500000000000002</v>
       </c>
-      <c r="AM38" s="57">
+      <c r="AM38" s="49">
         <v>0</v>
       </c>
     </row>
@@ -5115,17 +5110,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI39" s="56">
+      <c r="AI39" s="48">
         <v>0.53</v>
       </c>
-      <c r="AJ39" s="57">
+      <c r="AJ39" s="49">
         <v>0</v>
       </c>
-      <c r="AK39" s="55"/>
-      <c r="AL39" s="56">
+      <c r="AK39" s="47"/>
+      <c r="AL39" s="48">
         <v>0.53</v>
       </c>
-      <c r="AM39" s="57">
+      <c r="AM39" s="49">
         <v>0</v>
       </c>
     </row>
@@ -5200,17 +5195,17 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AI40" s="56">
+      <c r="AI40" s="48">
         <v>0.53500000000000003</v>
       </c>
-      <c r="AJ40" s="57">
+      <c r="AJ40" s="49">
         <v>0</v>
       </c>
-      <c r="AK40" s="55"/>
-      <c r="AL40" s="56">
+      <c r="AK40" s="47"/>
+      <c r="AL40" s="48">
         <v>0.53500000000000003</v>
       </c>
-      <c r="AM40" s="57">
+      <c r="AM40" s="49">
         <v>0</v>
       </c>
     </row>
@@ -5285,17 +5280,17 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="AI41" s="56">
+      <c r="AI41" s="48">
         <v>0.54</v>
       </c>
-      <c r="AJ41" s="57">
+      <c r="AJ41" s="49">
         <v>0</v>
       </c>
-      <c r="AK41" s="55"/>
-      <c r="AL41" s="56">
+      <c r="AK41" s="47"/>
+      <c r="AL41" s="48">
         <v>0.54</v>
       </c>
-      <c r="AM41" s="57">
+      <c r="AM41" s="49">
         <v>0</v>
       </c>
     </row>
@@ -5370,17 +5365,17 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="AI42" s="56">
+      <c r="AI42" s="48">
         <v>0.54500000000000004</v>
       </c>
-      <c r="AJ42" s="57">
+      <c r="AJ42" s="49">
         <v>0</v>
       </c>
-      <c r="AK42" s="55"/>
-      <c r="AL42" s="56">
+      <c r="AK42" s="47"/>
+      <c r="AL42" s="48">
         <v>0.54500000000000004</v>
       </c>
-      <c r="AM42" s="57">
+      <c r="AM42" s="49">
         <v>8</v>
       </c>
     </row>
@@ -5455,17 +5450,17 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="AI43" s="56">
+      <c r="AI43" s="48">
         <v>0.55000000000000004</v>
       </c>
-      <c r="AJ43" s="57">
+      <c r="AJ43" s="49">
         <v>0</v>
       </c>
-      <c r="AK43" s="55"/>
-      <c r="AL43" s="56">
+      <c r="AK43" s="47"/>
+      <c r="AL43" s="48">
         <v>0.55000000000000004</v>
       </c>
-      <c r="AM43" s="57">
+      <c r="AM43" s="49">
         <v>10</v>
       </c>
     </row>
@@ -5540,17 +5535,17 @@
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="AI44" s="56">
+      <c r="AI44" s="48">
         <v>0.55500000000000005</v>
       </c>
-      <c r="AJ44" s="57">
+      <c r="AJ44" s="49">
         <v>0</v>
       </c>
-      <c r="AK44" s="55"/>
-      <c r="AL44" s="56">
+      <c r="AK44" s="47"/>
+      <c r="AL44" s="48">
         <v>0.55500000000000005</v>
       </c>
-      <c r="AM44" s="57">
+      <c r="AM44" s="49">
         <v>36</v>
       </c>
     </row>
@@ -5625,17 +5620,17 @@
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
-      <c r="AI45" s="56">
+      <c r="AI45" s="48">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AJ45" s="57">
+      <c r="AJ45" s="49">
         <v>0</v>
       </c>
-      <c r="AK45" s="55"/>
-      <c r="AL45" s="56">
+      <c r="AK45" s="47"/>
+      <c r="AL45" s="48">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AM45" s="57">
+      <c r="AM45" s="49">
         <v>28</v>
       </c>
     </row>
@@ -5710,17 +5705,17 @@
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="AI46" s="56">
+      <c r="AI46" s="48">
         <v>0.56499999999999995</v>
       </c>
-      <c r="AJ46" s="57">
+      <c r="AJ46" s="49">
         <v>0</v>
       </c>
-      <c r="AK46" s="55"/>
-      <c r="AL46" s="56">
+      <c r="AK46" s="47"/>
+      <c r="AL46" s="48">
         <v>0.56499999999999995</v>
       </c>
-      <c r="AM46" s="57">
+      <c r="AM46" s="49">
         <v>24</v>
       </c>
     </row>
@@ -5795,17 +5790,17 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="AI47" s="56">
+      <c r="AI47" s="48">
         <v>0.56999999999999995</v>
       </c>
-      <c r="AJ47" s="57">
+      <c r="AJ47" s="49">
         <v>0</v>
       </c>
-      <c r="AK47" s="55"/>
-      <c r="AL47" s="56">
+      <c r="AK47" s="47"/>
+      <c r="AL47" s="48">
         <v>0.56999999999999995</v>
       </c>
-      <c r="AM47" s="57">
+      <c r="AM47" s="49">
         <v>6</v>
       </c>
     </row>
@@ -5880,17 +5875,17 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AI48" s="56">
+      <c r="AI48" s="48">
         <v>0.57499999999999996</v>
       </c>
-      <c r="AJ48" s="57">
+      <c r="AJ48" s="49">
         <v>0</v>
       </c>
-      <c r="AK48" s="55"/>
-      <c r="AL48" s="56">
+      <c r="AK48" s="47"/>
+      <c r="AL48" s="48">
         <v>0.57499999999999996</v>
       </c>
-      <c r="AM48" s="57">
+      <c r="AM48" s="49">
         <v>0</v>
       </c>
     </row>
@@ -5965,17 +5960,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI49" s="56">
+      <c r="AI49" s="48">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AJ49" s="57">
+      <c r="AJ49" s="49">
         <v>0</v>
       </c>
-      <c r="AK49" s="55"/>
-      <c r="AL49" s="56">
+      <c r="AK49" s="47"/>
+      <c r="AL49" s="48">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AM49" s="57">
+      <c r="AM49" s="49">
         <v>0</v>
       </c>
     </row>
@@ -6049,17 +6044,17 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AI50" s="56">
+      <c r="AI50" s="48">
         <v>0.58499999999999996</v>
       </c>
-      <c r="AJ50" s="57">
+      <c r="AJ50" s="49">
         <v>0</v>
       </c>
-      <c r="AK50" s="55"/>
-      <c r="AL50" s="56">
+      <c r="AK50" s="47"/>
+      <c r="AL50" s="48">
         <v>0.58499999999999996</v>
       </c>
-      <c r="AM50" s="57">
+      <c r="AM50" s="49">
         <v>0</v>
       </c>
     </row>
@@ -6133,17 +6128,17 @@
         <f>COUNTIF($J$19:$J$165, "&gt;="&amp;$AC51)-COUNTIF($J$19:$J$165,"&gt;=0.590")</f>
         <v>0</v>
       </c>
-      <c r="AI51" s="58" t="s">
+      <c r="AI51" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="AJ51" s="58">
+      <c r="AJ51" s="50">
         <v>0</v>
       </c>
-      <c r="AK51" s="55"/>
-      <c r="AL51" s="58" t="s">
+      <c r="AK51" s="47"/>
+      <c r="AL51" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="AM51" s="58">
+      <c r="AM51" s="50">
         <v>0</v>
       </c>
     </row>
@@ -12439,24 +12434,24 @@
       <c r="C132" t="s">
         <v>171</v>
       </c>
-      <c r="E132" s="47">
+      <c r="E132" s="41">
         <v>3</v>
       </c>
       <c r="F132" t="s">
         <v>65</v>
       </c>
-      <c r="H132" s="48">
+      <c r="H132" s="42">
         <v>0.54500000000000004</v>
       </c>
-      <c r="I132" s="48">
+      <c r="I132" s="42">
         <v>0.52500000000000002</v>
       </c>
-      <c r="J132" s="48">
+      <c r="J132" s="42">
         <v>0.54500000000000004</v>
       </c>
-      <c r="L132" s="48"/>
-      <c r="M132" s="48"/>
-      <c r="N132" s="48"/>
+      <c r="L132" s="42"/>
+      <c r="M132" s="42"/>
+      <c r="N132" s="42"/>
       <c r="P132" t="str">
         <f>IF(AND(J132&lt;=Constants!F$5,J132&gt;=Constants!E$5),"Y","N")</f>
         <v>N</v>
@@ -12509,24 +12504,24 @@
       <c r="C133" t="s">
         <v>172</v>
       </c>
-      <c r="E133" s="47">
+      <c r="E133" s="41">
         <v>3</v>
       </c>
       <c r="F133" t="s">
         <v>65</v>
       </c>
-      <c r="H133" s="48">
+      <c r="H133" s="42">
         <v>0.55700000000000005</v>
       </c>
-      <c r="I133" s="48">
+      <c r="I133" s="42">
         <v>0.53100000000000003</v>
       </c>
-      <c r="J133" s="48">
+      <c r="J133" s="42">
         <v>0.53100000000000003</v>
       </c>
-      <c r="L133" s="48"/>
-      <c r="M133" s="48"/>
-      <c r="N133" s="48"/>
+      <c r="L133" s="42"/>
+      <c r="M133" s="42"/>
+      <c r="N133" s="42"/>
       <c r="P133" t="str">
         <f>IF(AND(J133&lt;=Constants!F$5,J133&gt;=Constants!E$5),"Y","N")</f>
         <v>N</v>
@@ -12579,28 +12574,28 @@
       <c r="C134" t="s">
         <v>87</v>
       </c>
-      <c r="E134" s="47">
+      <c r="E134" s="41">
         <v>2</v>
       </c>
       <c r="F134" t="s">
         <v>65</v>
       </c>
-      <c r="H134" s="48">
+      <c r="H134" s="42">
         <v>0.57499999999999996</v>
       </c>
-      <c r="I134" s="48">
+      <c r="I134" s="42">
         <v>0.53500000000000003</v>
       </c>
-      <c r="J134" s="48">
+      <c r="J134" s="42">
         <v>0.53500000000000003</v>
       </c>
-      <c r="L134" s="48">
+      <c r="L134" s="42">
         <v>0.46700000000000003</v>
       </c>
-      <c r="M134" s="48">
+      <c r="M134" s="42">
         <v>0.435</v>
       </c>
-      <c r="N134" s="48">
+      <c r="N134" s="42">
         <v>0.435</v>
       </c>
       <c r="P134" t="str">
@@ -12613,7 +12608,7 @@
       </c>
       <c r="R134" t="str">
         <f>IF(AND(J134&lt;=Constants!F$7,J134&gt;=Constants!E$7),"Y","N")</f>
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="S134" t="str">
         <f>IF(P134="N","N",IF(OR((J134+Constants!D$14)&gt;Constants!F$5,(J134-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
@@ -12625,7 +12620,7 @@
       </c>
       <c r="U134" t="str">
         <f>IF(R134="N","N",IF(OR((J134+Constants!D$14)&gt;Constants!F$7,(J134-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="W134">
         <f>J134/2+Constants!D$9-Constants!D$10</f>
@@ -12655,28 +12650,28 @@
       <c r="C135" t="s">
         <v>174</v>
       </c>
-      <c r="E135" s="47">
+      <c r="E135" s="41">
         <v>2</v>
       </c>
       <c r="F135" t="s">
         <v>65</v>
       </c>
-      <c r="H135" s="48">
+      <c r="H135" s="42">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I135" s="48">
+      <c r="I135" s="42">
         <v>0.55300000000000005</v>
       </c>
-      <c r="J135" s="48">
+      <c r="J135" s="42">
         <v>0.55300000000000005</v>
       </c>
-      <c r="L135" s="48">
+      <c r="L135" s="42">
         <v>0.45300000000000001</v>
       </c>
-      <c r="M135" s="48">
+      <c r="M135" s="42">
         <v>0.441</v>
       </c>
-      <c r="N135" s="48">
+      <c r="N135" s="42">
         <v>0.441</v>
       </c>
       <c r="P135" t="str">
@@ -12731,28 +12726,28 @@
       <c r="C136" t="s">
         <v>82</v>
       </c>
-      <c r="E136" s="47">
+      <c r="E136" s="41">
         <v>3</v>
       </c>
       <c r="F136" t="s">
         <v>65</v>
       </c>
-      <c r="H136" s="48">
+      <c r="H136" s="42">
         <v>0.56399999999999995</v>
       </c>
-      <c r="I136" s="48">
+      <c r="I136" s="42">
         <v>0.56299999999999994</v>
       </c>
-      <c r="J136" s="48">
+      <c r="J136" s="42">
         <v>0.56299999999999994</v>
       </c>
-      <c r="L136" s="48">
+      <c r="L136" s="42">
         <v>0.47499999999999998</v>
       </c>
-      <c r="M136" s="48">
+      <c r="M136" s="42">
         <v>0.44800000000000001</v>
       </c>
-      <c r="N136" s="48">
+      <c r="N136" s="42">
         <v>0.44800000000000001</v>
       </c>
       <c r="P136" t="str">
@@ -12807,28 +12802,28 @@
       <c r="C137" t="s">
         <v>79</v>
       </c>
-      <c r="E137" s="47">
+      <c r="E137" s="41">
         <v>2</v>
       </c>
       <c r="F137" t="s">
         <v>65</v>
       </c>
-      <c r="H137" s="48">
+      <c r="H137" s="42">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I137" s="48">
+      <c r="I137" s="42">
         <v>0.54700000000000004</v>
       </c>
-      <c r="J137" s="48">
+      <c r="J137" s="42">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L137" s="48">
+      <c r="L137" s="42">
         <v>0.46700000000000003</v>
       </c>
-      <c r="M137" s="48">
+      <c r="M137" s="42">
         <v>0.442</v>
       </c>
-      <c r="N137" s="48">
+      <c r="N137" s="42">
         <v>0.442</v>
       </c>
       <c r="P137" t="str">
@@ -12883,28 +12878,28 @@
       <c r="C138" t="s">
         <v>175</v>
       </c>
-      <c r="E138" s="47">
+      <c r="E138" s="41">
         <v>2</v>
       </c>
       <c r="F138" t="s">
         <v>95</v>
       </c>
-      <c r="H138" s="48">
+      <c r="H138" s="42">
         <v>0.56399999999999995</v>
       </c>
-      <c r="I138" s="48">
+      <c r="I138" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="J138" s="48">
+      <c r="J138" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="L138" s="48">
+      <c r="L138" s="42">
         <v>0.45600000000000002</v>
       </c>
-      <c r="M138" s="48">
+      <c r="M138" s="42">
         <v>0.44500000000000001</v>
       </c>
-      <c r="N138" s="48">
+      <c r="N138" s="42">
         <v>0.44500000000000001</v>
       </c>
       <c r="P138" t="str">
@@ -12959,28 +12954,28 @@
       <c r="C139" t="s">
         <v>176</v>
       </c>
-      <c r="E139" s="47">
+      <c r="E139" s="41">
         <v>3</v>
       </c>
       <c r="F139" t="s">
         <v>65</v>
       </c>
-      <c r="H139" s="48">
+      <c r="H139" s="42">
         <v>0.55200000000000005</v>
       </c>
-      <c r="I139" s="48">
+      <c r="I139" s="42">
         <v>0.53500000000000003</v>
       </c>
-      <c r="J139" s="48">
+      <c r="J139" s="42">
         <v>0.55200000000000005</v>
       </c>
-      <c r="L139" s="48">
+      <c r="L139" s="42">
         <v>0.44</v>
       </c>
-      <c r="M139" s="48">
+      <c r="M139" s="42">
         <v>0.438</v>
       </c>
-      <c r="N139" s="48">
+      <c r="N139" s="42">
         <v>0.438</v>
       </c>
       <c r="P139" t="str">
@@ -13035,28 +13030,28 @@
       <c r="C140" t="s">
         <v>177</v>
       </c>
-      <c r="E140" s="47">
+      <c r="E140" s="41">
         <v>3</v>
       </c>
       <c r="F140" t="s">
         <v>65</v>
       </c>
-      <c r="H140" s="48">
+      <c r="H140" s="42">
         <v>0.56200000000000006</v>
       </c>
-      <c r="I140" s="48">
+      <c r="I140" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="J140" s="48">
+      <c r="J140" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="L140" s="48">
+      <c r="L140" s="42">
         <v>0.47399999999999998</v>
       </c>
-      <c r="M140" s="48">
+      <c r="M140" s="42">
         <v>0.44700000000000001</v>
       </c>
-      <c r="N140" s="48">
+      <c r="N140" s="42">
         <v>0.44700000000000001</v>
       </c>
       <c r="P140" t="str">
@@ -13111,28 +13106,28 @@
       <c r="C141" t="s">
         <v>178</v>
       </c>
-      <c r="E141" s="47">
+      <c r="E141" s="41">
         <v>2</v>
       </c>
       <c r="F141" t="s">
         <v>65</v>
       </c>
-      <c r="H141" s="48">
+      <c r="H141" s="42">
         <v>0.55400000000000005</v>
       </c>
-      <c r="I141" s="48">
+      <c r="I141" s="42">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J141" s="48">
+      <c r="J141" s="42">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L141" s="48">
+      <c r="L141" s="42">
         <v>0.47299999999999998</v>
       </c>
-      <c r="M141" s="48">
+      <c r="M141" s="42">
         <v>0.439</v>
       </c>
-      <c r="N141" s="48">
+      <c r="N141" s="42">
         <v>0.439</v>
       </c>
       <c r="P141" t="str">
@@ -13187,28 +13182,28 @@
       <c r="C142" t="s">
         <v>179</v>
       </c>
-      <c r="E142" s="47">
+      <c r="E142" s="41">
         <v>3</v>
       </c>
       <c r="F142" t="s">
         <v>65</v>
       </c>
-      <c r="H142" s="48">
+      <c r="H142" s="42">
         <v>0.57899999999999996</v>
       </c>
-      <c r="I142" s="48">
+      <c r="I142" s="42">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J142" s="48">
+      <c r="J142" s="42">
         <v>0.56999999999999995</v>
       </c>
-      <c r="L142" s="48">
+      <c r="L142" s="42">
         <v>0.47799999999999998</v>
       </c>
-      <c r="M142" s="48">
+      <c r="M142" s="42">
         <v>0.43</v>
       </c>
-      <c r="N142" s="48">
+      <c r="N142" s="42">
         <v>0.43</v>
       </c>
       <c r="P142" t="str">
@@ -13263,28 +13258,28 @@
       <c r="C143" t="s">
         <v>180</v>
       </c>
-      <c r="E143" s="47">
+      <c r="E143" s="41">
         <v>2</v>
       </c>
       <c r="F143" t="s">
         <v>95</v>
       </c>
-      <c r="H143" s="48">
+      <c r="H143" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="I143" s="48">
+      <c r="I143" s="42">
         <v>0.54900000000000004</v>
       </c>
-      <c r="J143" s="48">
+      <c r="J143" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="L143" s="48">
+      <c r="L143" s="42">
         <v>0.442</v>
       </c>
-      <c r="M143" s="48">
+      <c r="M143" s="42">
         <v>0.44</v>
       </c>
-      <c r="N143" s="48">
+      <c r="N143" s="42">
         <v>0.442</v>
       </c>
       <c r="P143" t="str">
@@ -13339,7 +13334,7 @@
       <c r="C144" t="s">
         <v>181</v>
       </c>
-      <c r="E144" s="47">
+      <c r="E144" s="41">
         <v>2</v>
       </c>
       <c r="F144" t="s">
@@ -13348,19 +13343,19 @@
       <c r="H144">
         <v>0.55700000000000005</v>
       </c>
-      <c r="I144" s="48">
+      <c r="I144" s="42">
         <v>0.54700000000000004</v>
       </c>
-      <c r="J144" s="48">
+      <c r="J144" s="42">
         <v>0.54700000000000004</v>
       </c>
-      <c r="L144" s="48">
+      <c r="L144" s="42">
         <v>0.44700000000000001</v>
       </c>
-      <c r="M144" s="48">
+      <c r="M144" s="42">
         <v>0.441</v>
       </c>
-      <c r="N144" s="48">
+      <c r="N144" s="42">
         <v>0.441</v>
       </c>
       <c r="P144" t="str">
@@ -13415,28 +13410,28 @@
       <c r="C145" t="s">
         <v>182</v>
       </c>
-      <c r="E145" s="47">
+      <c r="E145" s="41">
         <v>2</v>
       </c>
       <c r="F145" t="s">
         <v>65</v>
       </c>
-      <c r="H145" s="48">
+      <c r="H145" s="42">
         <v>0.55200000000000005</v>
       </c>
-      <c r="I145" s="48">
+      <c r="I145" s="42">
         <v>0.54</v>
       </c>
-      <c r="J145" s="48">
+      <c r="J145" s="42">
         <v>0.55200000000000005</v>
       </c>
-      <c r="L145" s="48">
+      <c r="L145" s="42">
         <v>0.46300000000000002</v>
       </c>
-      <c r="M145" s="48">
+      <c r="M145" s="42">
         <v>0.44</v>
       </c>
-      <c r="N145" s="48">
+      <c r="N145" s="42">
         <v>0.44</v>
       </c>
       <c r="P145" t="str">
@@ -13491,28 +13486,28 @@
       <c r="C146" t="s">
         <v>183</v>
       </c>
-      <c r="E146" s="47">
+      <c r="E146" s="41">
         <v>3</v>
       </c>
       <c r="F146" t="s">
         <v>65</v>
       </c>
-      <c r="H146" s="48">
+      <c r="H146" s="42">
         <v>0.55500000000000005</v>
       </c>
-      <c r="I146" s="48">
+      <c r="I146" s="42">
         <v>0.54600000000000004</v>
       </c>
-      <c r="J146" s="48">
+      <c r="J146" s="42">
         <v>0.55500000000000005</v>
       </c>
-      <c r="L146" s="48">
+      <c r="L146" s="42">
         <v>0.44500000000000001</v>
       </c>
-      <c r="M146" s="48">
+      <c r="M146" s="42">
         <v>0.442</v>
       </c>
-      <c r="N146" s="48">
+      <c r="N146" s="42">
         <v>0.442</v>
       </c>
       <c r="P146" t="str">
@@ -13567,28 +13562,28 @@
       <c r="C147" t="s">
         <v>184</v>
       </c>
-      <c r="E147" s="47">
+      <c r="E147" s="41">
         <v>3</v>
       </c>
       <c r="F147" t="s">
         <v>95</v>
       </c>
-      <c r="H147" s="48">
+      <c r="H147" s="42">
         <v>0.55600000000000005</v>
       </c>
-      <c r="I147" s="48">
+      <c r="I147" s="42">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J147" s="48">
+      <c r="J147" s="42">
         <v>0.55600000000000005</v>
       </c>
-      <c r="L147" s="48">
+      <c r="L147" s="42">
         <v>0.443</v>
       </c>
-      <c r="M147" s="48">
+      <c r="M147" s="42">
         <v>0.44</v>
       </c>
-      <c r="N147" s="48">
+      <c r="N147" s="42">
         <v>0.44</v>
       </c>
       <c r="P147" t="str">
@@ -13643,28 +13638,28 @@
       <c r="C148" t="s">
         <v>185</v>
       </c>
-      <c r="E148" s="47">
+      <c r="E148" s="41">
         <v>2</v>
       </c>
       <c r="F148" t="s">
         <v>95</v>
       </c>
-      <c r="H148" s="48">
+      <c r="H148" s="42">
         <v>0.56699999999999995</v>
       </c>
-      <c r="I148" s="48">
+      <c r="I148" s="42">
         <v>0.55900000000000005</v>
       </c>
-      <c r="J148" s="48">
+      <c r="J148" s="42">
         <v>0.55900000000000005</v>
       </c>
-      <c r="L148" s="48">
+      <c r="L148" s="42">
         <v>0.46</v>
       </c>
-      <c r="M148" s="48">
+      <c r="M148" s="42">
         <v>0.44600000000000001</v>
       </c>
-      <c r="N148" s="48">
+      <c r="N148" s="42">
         <v>0.44600000000000001</v>
       </c>
       <c r="P148" t="str">
@@ -13719,28 +13714,28 @@
       <c r="C149" t="s">
         <v>186</v>
       </c>
-      <c r="E149" s="47">
+      <c r="E149" s="41">
         <v>3</v>
       </c>
       <c r="F149" t="s">
         <v>65</v>
       </c>
-      <c r="H149" s="48">
+      <c r="H149" s="42">
         <v>0.56499999999999995</v>
       </c>
-      <c r="I149" s="48">
+      <c r="I149" s="42">
         <v>0.55500000000000005</v>
       </c>
-      <c r="J149" s="48">
+      <c r="J149" s="42">
         <v>0.55500000000000005</v>
       </c>
-      <c r="L149" s="48">
+      <c r="L149" s="42">
         <v>0.47199999999999998</v>
       </c>
-      <c r="M149" s="48">
+      <c r="M149" s="42">
         <v>0.44400000000000001</v>
       </c>
-      <c r="N149" s="48">
+      <c r="N149" s="42">
         <v>0.44400000000000001</v>
       </c>
       <c r="P149" t="str">
@@ -13795,28 +13790,28 @@
       <c r="C150" t="s">
         <v>187</v>
       </c>
-      <c r="E150" s="47">
+      <c r="E150" s="41">
         <v>2</v>
       </c>
       <c r="F150" t="s">
         <v>95</v>
       </c>
-      <c r="H150" s="48">
+      <c r="H150" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="I150" s="48">
+      <c r="I150" s="42">
         <v>0.54700000000000004</v>
       </c>
-      <c r="J150" s="48">
+      <c r="J150" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="L150" s="48">
+      <c r="L150" s="42">
         <v>0.44</v>
       </c>
-      <c r="M150" s="48">
+      <c r="M150" s="42">
         <v>0.437</v>
       </c>
-      <c r="N150" s="48">
+      <c r="N150" s="42">
         <v>0.437</v>
       </c>
       <c r="P150" t="str">
@@ -13871,28 +13866,28 @@
       <c r="C151" t="s">
         <v>188</v>
       </c>
-      <c r="E151" s="47">
+      <c r="E151" s="41">
         <v>2</v>
       </c>
       <c r="F151" t="s">
         <v>95</v>
       </c>
-      <c r="H151" s="48">
+      <c r="H151" s="42">
         <v>0.56399999999999995</v>
       </c>
-      <c r="I151" s="48">
+      <c r="I151" s="42">
         <v>0.55500000000000005</v>
       </c>
-      <c r="J151" s="48">
+      <c r="J151" s="42">
         <v>0.56399999999999995</v>
       </c>
-      <c r="L151" s="48">
+      <c r="L151" s="42">
         <v>0.44900000000000001</v>
       </c>
-      <c r="M151" s="48">
+      <c r="M151" s="42">
         <v>0.441</v>
       </c>
-      <c r="N151" s="48">
+      <c r="N151" s="42">
         <v>0.441</v>
       </c>
       <c r="P151" t="str">
@@ -13947,28 +13942,28 @@
       <c r="C152" t="s">
         <v>189</v>
       </c>
-      <c r="E152" s="47">
+      <c r="E152" s="41">
         <v>2</v>
       </c>
       <c r="F152" t="s">
         <v>65</v>
       </c>
-      <c r="H152" s="48">
+      <c r="H152" s="42">
         <v>0.55400000000000005</v>
       </c>
-      <c r="I152" s="48">
+      <c r="I152" s="42">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J152" s="48">
+      <c r="J152" s="42">
         <v>0.55400000000000005</v>
       </c>
-      <c r="L152" s="48">
+      <c r="L152" s="42">
         <v>0.45100000000000001</v>
       </c>
-      <c r="M152" s="48">
+      <c r="M152" s="42">
         <v>0.441</v>
       </c>
-      <c r="N152" s="48">
+      <c r="N152" s="42">
         <v>0.441</v>
       </c>
       <c r="P152" t="str">
@@ -14023,28 +14018,28 @@
       <c r="C153" t="s">
         <v>190</v>
       </c>
-      <c r="E153" s="47">
+      <c r="E153" s="41">
         <v>3</v>
       </c>
       <c r="F153" t="s">
         <v>65</v>
       </c>
-      <c r="H153" s="48">
+      <c r="H153" s="42">
         <v>0.55500000000000005</v>
       </c>
-      <c r="I153" s="48">
+      <c r="I153" s="42">
         <v>0.54300000000000004</v>
       </c>
-      <c r="J153" s="48">
+      <c r="J153" s="42">
         <v>0.55500000000000005</v>
       </c>
-      <c r="L153" s="48">
+      <c r="L153" s="42">
         <v>0.45</v>
       </c>
-      <c r="M153" s="48">
+      <c r="M153" s="42">
         <v>0.44</v>
       </c>
-      <c r="N153" s="48">
+      <c r="N153" s="42">
         <v>0.44</v>
       </c>
       <c r="P153" t="str">
@@ -14099,28 +14094,28 @@
       <c r="C154" t="s">
         <v>191</v>
       </c>
-      <c r="E154" s="47">
+      <c r="E154" s="41">
         <v>3</v>
       </c>
       <c r="F154" t="s">
         <v>65</v>
       </c>
-      <c r="H154" s="48">
+      <c r="H154" s="42">
         <v>0.55200000000000005</v>
       </c>
-      <c r="I154" s="48">
+      <c r="I154" s="42">
         <v>0.53500000000000003</v>
       </c>
-      <c r="J154" s="48">
+      <c r="J154" s="42">
         <v>0.55200000000000005</v>
       </c>
-      <c r="L154" s="48">
+      <c r="L154" s="42">
         <v>0.45900000000000002</v>
       </c>
-      <c r="M154" s="48">
+      <c r="M154" s="42">
         <v>0.441</v>
       </c>
-      <c r="N154" s="48">
+      <c r="N154" s="42">
         <v>0.441</v>
       </c>
       <c r="P154" t="str">
@@ -14175,28 +14170,28 @@
       <c r="C155" t="s">
         <v>192</v>
       </c>
-      <c r="E155" s="47">
+      <c r="E155" s="41">
         <v>2</v>
       </c>
       <c r="F155" t="s">
         <v>95</v>
       </c>
-      <c r="H155" s="48">
+      <c r="H155" s="42">
         <v>0.55700000000000005</v>
       </c>
-      <c r="I155" s="48">
+      <c r="I155" s="42">
         <v>0.54600000000000004</v>
       </c>
-      <c r="J155" s="48">
+      <c r="J155" s="42">
         <v>0.55700000000000005</v>
       </c>
-      <c r="L155" s="48">
+      <c r="L155" s="42">
         <v>0.443</v>
       </c>
-      <c r="M155" s="48">
+      <c r="M155" s="42">
         <v>0.442</v>
       </c>
-      <c r="N155" s="48">
+      <c r="N155" s="42">
         <v>0.442</v>
       </c>
       <c r="P155" t="str">
@@ -14251,28 +14246,28 @@
       <c r="C156" t="s">
         <v>193</v>
       </c>
-      <c r="E156" s="47">
+      <c r="E156" s="41">
         <v>2</v>
       </c>
       <c r="F156" t="s">
         <v>65</v>
       </c>
-      <c r="H156" s="48">
+      <c r="H156" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="I156" s="48">
+      <c r="I156" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="J156" s="48">
+      <c r="J156" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="L156" s="48">
+      <c r="L156" s="42">
         <v>0.45500000000000002</v>
       </c>
-      <c r="M156" s="48">
+      <c r="M156" s="42">
         <v>0.44400000000000001</v>
       </c>
-      <c r="N156" s="48">
+      <c r="N156" s="42">
         <v>0.44400000000000001</v>
       </c>
       <c r="P156" t="str">
@@ -14327,28 +14322,28 @@
       <c r="C157" t="s">
         <v>194</v>
       </c>
-      <c r="E157" s="47">
+      <c r="E157" s="41">
         <v>2</v>
       </c>
       <c r="F157" t="s">
         <v>65</v>
       </c>
-      <c r="H157" s="48">
+      <c r="H157" s="42">
         <v>0.55600000000000005</v>
       </c>
-      <c r="I157" s="48">
+      <c r="I157" s="42">
         <v>0.54800000000000004</v>
       </c>
-      <c r="J157" s="48">
+      <c r="J157" s="42">
         <v>0.55600000000000005</v>
       </c>
-      <c r="L157" s="48">
+      <c r="L157" s="42">
         <v>0.44900000000000001</v>
       </c>
-      <c r="M157" s="48">
+      <c r="M157" s="42">
         <v>0.432</v>
       </c>
-      <c r="N157" s="48">
+      <c r="N157" s="42">
         <v>0.432</v>
       </c>
       <c r="P157" t="str">
@@ -14403,28 +14398,28 @@
       <c r="C158" t="s">
         <v>195</v>
       </c>
-      <c r="E158" s="47">
+      <c r="E158" s="41">
         <v>2</v>
       </c>
       <c r="F158" t="s">
         <v>65</v>
       </c>
-      <c r="H158" s="48">
+      <c r="H158" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="I158" s="48">
+      <c r="I158" s="42">
         <v>0.55400000000000005</v>
       </c>
-      <c r="J158" s="48">
+      <c r="J158" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="L158" s="48">
+      <c r="L158" s="42">
         <v>0.44900000000000001</v>
       </c>
-      <c r="M158" s="48">
+      <c r="M158" s="42">
         <v>0.443</v>
       </c>
-      <c r="N158" s="48">
+      <c r="N158" s="42">
         <v>0.443</v>
       </c>
       <c r="P158" t="str">
@@ -14479,28 +14474,28 @@
       <c r="C159" t="s">
         <v>196</v>
       </c>
-      <c r="E159" s="47">
+      <c r="E159" s="41">
         <v>2</v>
       </c>
       <c r="F159" t="s">
         <v>65</v>
       </c>
-      <c r="H159" s="48">
+      <c r="H159" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="I159" s="48">
+      <c r="I159" s="42">
         <v>0.53900000000000003</v>
       </c>
-      <c r="J159" s="48">
+      <c r="J159" s="42">
         <v>0.53900000000000003</v>
       </c>
-      <c r="L159" s="48">
+      <c r="L159" s="42">
         <v>0.45500000000000002</v>
       </c>
-      <c r="M159" s="48">
+      <c r="M159" s="42">
         <v>0.435</v>
       </c>
-      <c r="N159" s="48">
+      <c r="N159" s="42">
         <v>0.435</v>
       </c>
       <c r="P159" t="str">
@@ -14525,7 +14520,7 @@
       </c>
       <c r="U159" t="str">
         <f>IF(R159="N","N",IF(OR((J159+Constants!D$14)&gt;Constants!F$7,(J159-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
-        <v>Y</v>
+        <v>Good</v>
       </c>
       <c r="W159">
         <f>J159/2+Constants!D$9-Constants!D$10</f>
@@ -14555,28 +14550,28 @@
       <c r="C160" t="s">
         <v>197</v>
       </c>
-      <c r="E160" s="47">
+      <c r="E160" s="41">
         <v>2</v>
       </c>
       <c r="F160" t="s">
         <v>65</v>
       </c>
-      <c r="H160" s="48">
+      <c r="H160" s="42">
         <v>0.55900000000000005</v>
       </c>
-      <c r="I160" s="48">
+      <c r="I160" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="J160" s="48">
+      <c r="J160" s="42">
         <v>0.55900000000000005</v>
       </c>
-      <c r="L160" s="48">
+      <c r="L160" s="42">
         <v>0.44700000000000001</v>
       </c>
-      <c r="M160" s="48">
+      <c r="M160" s="42">
         <v>0.435</v>
       </c>
-      <c r="N160" s="48">
+      <c r="N160" s="42">
         <v>0.435</v>
       </c>
       <c r="P160" t="str">
@@ -14631,28 +14626,28 @@
       <c r="C161" t="s">
         <v>198</v>
       </c>
-      <c r="E161" s="47">
+      <c r="E161" s="41">
         <v>2</v>
       </c>
       <c r="F161" t="s">
         <v>65</v>
       </c>
-      <c r="H161" s="48">
+      <c r="H161" s="42">
         <v>0.55300000000000005</v>
       </c>
-      <c r="I161" s="48">
+      <c r="I161" s="42">
         <v>0.54900000000000004</v>
       </c>
-      <c r="J161" s="48">
+      <c r="J161" s="42">
         <v>0.54900000000000004</v>
       </c>
-      <c r="L161" s="48">
+      <c r="L161" s="42">
         <v>0.46500000000000002</v>
       </c>
-      <c r="M161" s="48">
+      <c r="M161" s="42">
         <v>0.44700000000000001</v>
       </c>
-      <c r="N161" s="48">
+      <c r="N161" s="42">
         <v>0.44700000000000001</v>
       </c>
       <c r="P161" t="str">
@@ -14707,28 +14702,28 @@
       <c r="C162" t="s">
         <v>199</v>
       </c>
-      <c r="E162" s="47">
+      <c r="E162" s="41">
         <v>3</v>
       </c>
       <c r="F162" t="s">
         <v>65</v>
       </c>
-      <c r="H162" s="48">
+      <c r="H162" s="42">
         <v>0.56399999999999995</v>
       </c>
-      <c r="I162" s="48">
+      <c r="I162" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="J162" s="48">
+      <c r="J162" s="42">
         <v>0.55800000000000005</v>
       </c>
-      <c r="L162" s="48">
+      <c r="L162" s="42">
         <v>0.46</v>
       </c>
-      <c r="M162" s="48">
+      <c r="M162" s="42">
         <v>0.441</v>
       </c>
-      <c r="N162" s="48">
+      <c r="N162" s="42">
         <v>0.441</v>
       </c>
       <c r="P162" t="str">
@@ -14783,28 +14778,28 @@
       <c r="C163" t="s">
         <v>200</v>
       </c>
-      <c r="E163" s="47">
+      <c r="E163" s="41">
         <v>2</v>
       </c>
       <c r="F163" t="s">
         <v>65</v>
       </c>
-      <c r="H163" s="48">
+      <c r="H163" s="42">
         <v>0.56499999999999995</v>
       </c>
-      <c r="I163" s="48">
+      <c r="I163" s="42">
         <v>0.54300000000000004</v>
       </c>
-      <c r="J163" s="48">
+      <c r="J163" s="42">
         <v>0.54300000000000004</v>
       </c>
-      <c r="L163" s="48">
+      <c r="L163" s="42">
         <v>0.47399999999999998</v>
       </c>
-      <c r="M163" s="48">
+      <c r="M163" s="42">
         <v>0.439</v>
       </c>
-      <c r="N163" s="48">
+      <c r="N163" s="42">
         <v>0.439</v>
       </c>
       <c r="P163" t="str">
@@ -14859,28 +14854,28 @@
       <c r="C164" t="s">
         <v>138</v>
       </c>
-      <c r="E164" s="47">
+      <c r="E164" s="41">
         <v>2</v>
       </c>
       <c r="F164" t="s">
         <v>65</v>
       </c>
-      <c r="H164" s="48">
+      <c r="H164" s="42">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I164" s="48">
+      <c r="I164" s="42">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J164" s="48">
+      <c r="J164" s="42">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L164" s="48">
+      <c r="L164" s="42">
         <v>0.435</v>
       </c>
-      <c r="M164" s="48">
+      <c r="M164" s="42">
         <v>0.43</v>
       </c>
-      <c r="N164" s="48">
+      <c r="N164" s="42">
         <v>0.43</v>
       </c>
       <c r="P164" t="str">
@@ -14935,28 +14930,28 @@
       <c r="C165" t="s">
         <v>201</v>
       </c>
-      <c r="E165" s="47">
+      <c r="E165" s="41">
         <v>2</v>
       </c>
       <c r="F165" t="s">
         <v>65</v>
       </c>
-      <c r="H165" s="48">
+      <c r="H165" s="42">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I165" s="48">
+      <c r="I165" s="42">
         <v>0.55900000000000005</v>
       </c>
-      <c r="J165" s="48">
+      <c r="J165" s="42">
         <v>0.55900000000000005</v>
       </c>
-      <c r="L165" s="48">
+      <c r="L165" s="42">
         <v>0.45400000000000001</v>
       </c>
-      <c r="M165" s="48">
+      <c r="M165" s="42">
         <v>0.439</v>
       </c>
-      <c r="N165" s="48">
+      <c r="N165" s="42">
         <v>0.439</v>
       </c>
       <c r="P165" t="str">

</xml_diff>

<commit_message>
minor update in plug width
</commit_message>
<xml_diff>
--- a/data/PlugWidthEvaluation.xlsx
+++ b/data/PlugWidthEvaluation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="1" r:id="rId1"/>
@@ -1526,11 +1526,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="74446336"/>
-        <c:axId val="74448256"/>
+        <c:axId val="146535936"/>
+        <c:axId val="146537856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74446336"/>
+        <c:axId val="146535936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1559,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74448256"/>
+        <c:crossAx val="146537856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1567,7 +1567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74448256"/>
+        <c:axId val="146537856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,7 +1596,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74446336"/>
+        <c:crossAx val="146535936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1942,7 +1942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -3159,10 +3159,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A17:AM176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="16" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="16" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="Z10" sqref="Z10"/>
+      <selection pane="bottomLeft" activeCell="U133" sqref="U133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added leland data to plug width
</commit_message>
<xml_diff>
--- a/data/PlugWidthEvaluation.xlsx
+++ b/data/PlugWidthEvaluation.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="100" windowWidth="27800" windowHeight="14380"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="233">
   <si>
     <t>Plug</t>
   </si>
@@ -628,6 +633,93 @@
   </si>
   <si>
     <t>Less</t>
+  </si>
+  <si>
+    <t>4312 Leland</t>
+  </si>
+  <si>
+    <t>Lenovo charger</t>
+  </si>
+  <si>
+    <t>Old ass extension cord</t>
+  </si>
+  <si>
+    <t>Grounding plug</t>
+  </si>
+  <si>
+    <t>Macbook charger (bent straight manually)</t>
+  </si>
+  <si>
+    <t>Comcast box</t>
+  </si>
+  <si>
+    <t>Upstairs TV</t>
+  </si>
+  <si>
+    <t>DVD player</t>
+  </si>
+  <si>
+    <t>Amazon fire stick</t>
+  </si>
+  <si>
+    <t>Apple usb wall adapter (1''x 1'' white box)</t>
+  </si>
+  <si>
+    <t>Amazon basics wall adapter</t>
+  </si>
+  <si>
+    <t>Apple usb wall adapter</t>
+  </si>
+  <si>
+    <t>Phillips trimmer charger</t>
+  </si>
+  <si>
+    <t>Bose speakers</t>
+  </si>
+  <si>
+    <t>Philips sunrise alarm clock</t>
+  </si>
+  <si>
+    <t>4313 Leland</t>
+  </si>
+  <si>
+    <t>4314 Leland</t>
+  </si>
+  <si>
+    <t>4315 Leland</t>
+  </si>
+  <si>
+    <t>4316 Leland</t>
+  </si>
+  <si>
+    <t>4317 Leland</t>
+  </si>
+  <si>
+    <t>4318 Leland</t>
+  </si>
+  <si>
+    <t>4319 Leland</t>
+  </si>
+  <si>
+    <t>4320 Leland</t>
+  </si>
+  <si>
+    <t>4321 Leland</t>
+  </si>
+  <si>
+    <t>4322 Leland</t>
+  </si>
+  <si>
+    <t>4323 Leland</t>
+  </si>
+  <si>
+    <t>4324 Leland</t>
+  </si>
+  <si>
+    <t>4325 Leland</t>
+  </si>
+  <si>
+    <t>4326 Leland</t>
   </si>
 </sst>
 </file>
@@ -692,11 +784,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -705,7 +797,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -713,17 +805,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -733,7 +825,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -741,12 +833,12 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -755,31 +847,31 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -787,23 +879,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -811,7 +903,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -821,7 +913,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -829,20 +921,20 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -850,17 +942,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -870,7 +962,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -878,23 +970,23 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1090,13 +1182,13 @@
                   <c:v>0.41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41499999999999998</c:v>
+                  <c:v>0.415</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.42499999999999999</c:v>
+                  <c:v>0.425</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.43</c:v>
@@ -1108,79 +1200,79 @@
                   <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.44500000000000001</c:v>
+                  <c:v>0.445</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.45500000000000002</c:v>
+                  <c:v>0.455</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.46500000000000002</c:v>
+                  <c:v>0.465</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.47499999999999998</c:v>
+                  <c:v>0.475</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.48499999999999999</c:v>
+                  <c:v>0.485</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.51</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.51500000000000001</c:v>
+                  <c:v>0.515</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.52500000000000002</c:v>
+                  <c:v>0.525</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.53500000000000003</c:v>
+                  <c:v>0.535</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.54500000000000004</c:v>
+                  <c:v>0.545</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.55</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.55500000000000005</c:v>
+                  <c:v>0.555</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>0.56</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.56499999999999995</c:v>
+                  <c:v>0.565</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.56999999999999995</c:v>
+                  <c:v>0.57</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.57499999999999996</c:v>
+                  <c:v>0.575</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.58</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.58499999999999996</c:v>
+                  <c:v>0.585</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1192,100 +1284,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>33</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>52</c:v>
+                  <c:v>55.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>33</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1316,13 +1408,13 @@
                   <c:v>0.41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41499999999999998</c:v>
+                  <c:v>0.415</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.42499999999999999</c:v>
+                  <c:v>0.425</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.43</c:v>
@@ -1334,79 +1426,79 @@
                   <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.44500000000000001</c:v>
+                  <c:v>0.445</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.45500000000000002</c:v>
+                  <c:v>0.455</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.46500000000000002</c:v>
+                  <c:v>0.465</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.47499999999999998</c:v>
+                  <c:v>0.475</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.48499999999999999</c:v>
+                  <c:v>0.485</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.51</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.51500000000000001</c:v>
+                  <c:v>0.515</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.52500000000000002</c:v>
+                  <c:v>0.525</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.53500000000000003</c:v>
+                  <c:v>0.535</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.54500000000000004</c:v>
+                  <c:v>0.545</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.55</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.55500000000000005</c:v>
+                  <c:v>0.555</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>0.56</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.56499999999999995</c:v>
+                  <c:v>0.565</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.56999999999999995</c:v>
+                  <c:v>0.57</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.57499999999999996</c:v>
+                  <c:v>0.575</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.58</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.58499999999999996</c:v>
+                  <c:v>0.585</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1418,100 +1510,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29</c:v>
+                  <c:v>35.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43</c:v>
+                  <c:v>46.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1526,11 +1618,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="146535936"/>
-        <c:axId val="146537856"/>
+        <c:axId val="2141267128"/>
+        <c:axId val="2141260280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146535936"/>
+        <c:axId val="2141267128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1651,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146537856"/>
+        <c:crossAx val="2141260280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1567,7 +1659,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146537856"/>
+        <c:axId val="2141260280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,7 +1688,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146535936"/>
+        <c:crossAx val="2141267128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1942,20 +2034,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O166"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="9.140625" customWidth="1"/>
+    <col min="1" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="10"/>
@@ -1968,7 +2060,7 @@
       </c>
       <c r="K2" s="52"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15">
       <c r="B3" s="4" t="s">
         <v>48</v>
       </c>
@@ -1991,7 +2083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -2019,7 +2111,7 @@
         <v>67.500000000000057</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15">
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -2039,7 +2131,7 @@
         <v>0.60399999999999998</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15">
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -2059,7 +2151,7 @@
         <v>0.59399999999999997</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15">
       <c r="B7" s="31" t="s">
         <v>165</v>
       </c>
@@ -2079,10 +2171,10 @@
         <v>0.57799999999999996</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="15" thickBot="1">
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15">
       <c r="B9" s="1" t="s">
         <v>45</v>
       </c>
@@ -2099,11 +2191,11 @@
       <c r="K9" s="34"/>
       <c r="L9" s="34">
         <f>COUNT(Data!J19:J1000)</f>
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="M9" s="35"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15">
       <c r="B10" s="4" t="s">
         <v>46</v>
       </c>
@@ -2121,7 +2213,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15">
       <c r="B11" s="4" t="s">
         <v>47</v>
       </c>
@@ -2142,7 +2234,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15">
       <c r="B12" s="7" t="s">
         <v>152</v>
       </c>
@@ -2159,16 +2251,16 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5">
         <f>COUNTIF(Data!P19:P1000,"Y")</f>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="M12" s="37">
         <f>COUNTIF(Data!P19:P1000,"N")</f>
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2184,12 +2276,12 @@
       </c>
       <c r="M13" s="37">
         <f>L9-L13</f>
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15">
       <c r="B14" s="20" t="s">
         <v>157</v>
       </c>
@@ -2206,7 +2298,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15">
       <c r="H15" s="36"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -2216,7 +2308,7 @@
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15">
       <c r="B16" s="1" t="s">
         <v>70</v>
       </c>
@@ -2232,16 +2324,16 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5">
         <f>COUNTIF(Data!Q19:Q1000,"Y")</f>
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="M16" s="37">
         <f>COUNTIF(Data!Q19:Q1000,"N")</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15">
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="17">
@@ -2255,16 +2347,16 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5">
         <f>COUNTIF(Data!T19:T1000,"Good")</f>
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="M17" s="37">
         <f>L9-L17</f>
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15">
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="17">
@@ -2279,7 +2371,7 @@
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15">
       <c r="B19" s="4"/>
       <c r="C19" s="27"/>
       <c r="D19" s="17">
@@ -2293,7 +2385,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5">
         <f>COUNTIF(Data!R19:R1000,"Y")</f>
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="M19" s="37">
         <f>COUNTIF(Data!R19:R1000,"N")</f>
@@ -2302,7 +2394,7 @@
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
     </row>
-    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:15" ht="15" thickBot="1">
       <c r="B20" s="4"/>
       <c r="C20" s="27"/>
       <c r="D20" s="17">
@@ -2316,7 +2408,7 @@
       <c r="K20" s="39"/>
       <c r="L20" s="39">
         <f>COUNTIF(Data!U19:U1000,"Good")</f>
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="M20" s="40">
         <f>L9-L20</f>
@@ -2325,7 +2417,7 @@
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15">
       <c r="B21" s="4"/>
       <c r="C21" s="27"/>
       <c r="D21" s="17">
@@ -2340,7 +2432,7 @@
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15">
       <c r="B22" s="4"/>
       <c r="C22" s="27"/>
       <c r="D22" s="17">
@@ -2349,7 +2441,7 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15">
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="17">
@@ -2358,7 +2450,7 @@
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15">
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="17">
@@ -2367,7 +2459,7 @@
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15">
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="17">
@@ -2376,7 +2468,7 @@
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15">
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="17">
@@ -2385,7 +2477,7 @@
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15">
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="17">
@@ -2394,7 +2486,7 @@
       <c r="N27" s="11"/>
       <c r="O27" s="11"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15">
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="17">
@@ -2403,7 +2495,7 @@
       <c r="N28" s="11"/>
       <c r="O28" s="11"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15">
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
       <c r="D29" s="17">
@@ -2412,7 +2504,7 @@
       <c r="N29" s="11"/>
       <c r="O29" s="11"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15">
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
       <c r="D30" s="17">
@@ -2421,7 +2513,7 @@
       <c r="N30" s="11"/>
       <c r="O30" s="11"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15">
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
       <c r="D31" s="17">
@@ -2430,7 +2522,7 @@
       <c r="N31" s="11"/>
       <c r="O31" s="11"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15">
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
       <c r="D32" s="17">
@@ -2439,7 +2531,7 @@
       <c r="N32" s="11"/>
       <c r="O32" s="11"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15">
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="17">
@@ -2448,7 +2540,7 @@
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15">
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
       <c r="D34" s="17">
@@ -2457,7 +2549,7 @@
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15">
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
       <c r="D35" s="17">
@@ -2466,681 +2558,681 @@
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15">
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
       <c r="D36" s="17">
         <v>0.53</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15">
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
       <c r="D37" s="17">
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15">
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
       <c r="D38" s="17">
         <v>0.54</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15">
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="17">
         <v>0.54500000000000004</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15">
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
       <c r="D40" s="17">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15">
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
       <c r="D41" s="17">
         <v>0.55500000000000005</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15">
       <c r="B42" s="4"/>
       <c r="C42" s="5"/>
       <c r="D42" s="17">
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15">
       <c r="B43" s="4"/>
       <c r="C43" s="5"/>
       <c r="D43" s="17">
         <v>0.56499999999999995</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15">
       <c r="B44" s="4"/>
       <c r="C44" s="5"/>
       <c r="D44" s="17">
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15">
       <c r="B45" s="4"/>
       <c r="C45" s="5"/>
       <c r="D45" s="17">
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15">
       <c r="B46" s="4"/>
       <c r="C46" s="5"/>
       <c r="D46" s="17">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15">
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>
       <c r="D47" s="18">
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="14"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="14"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="14"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="14"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="14"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="14"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="14"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="14"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="14"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="14"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="14"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4">
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="14"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="14"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4">
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="14"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="14"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="14"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="14"/>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="14"/>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4">
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="14"/>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="14"/>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4">
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="14"/>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4">
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="14"/>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="14"/>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4">
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="14"/>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="14"/>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="14"/>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="14"/>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4">
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="14"/>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="14"/>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4">
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="14"/>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="14"/>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:4">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="14"/>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4">
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="14"/>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4">
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="14"/>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:4">
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="14"/>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:4">
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="14"/>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:4">
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="14"/>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:4">
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="14"/>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:4">
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="14"/>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:4">
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="14"/>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:4">
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="14"/>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:4">
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="14"/>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:4">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="14"/>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:4">
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="28"/>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:4">
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="28"/>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:4">
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="28"/>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:4">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="28"/>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:4">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="28"/>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:4">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="28"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:4">
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="28"/>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:4">
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="28"/>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:4">
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="28"/>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:4">
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="28"/>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:4">
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
       <c r="D101" s="28"/>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:4">
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="28"/>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:4">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="28"/>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:4">
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="28"/>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:4">
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="28"/>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:4">
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
       <c r="D106" s="28"/>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:4">
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
       <c r="D107" s="28"/>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:4">
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
       <c r="D108" s="28"/>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:4">
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="28"/>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:4">
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="28"/>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:4">
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="28"/>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:4">
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="28"/>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:4">
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="28"/>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:4">
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
       <c r="D114" s="28"/>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:4">
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
       <c r="D115" s="28"/>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:4">
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
       <c r="D116" s="28"/>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:4">
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
       <c r="D117" s="28"/>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:4">
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
       <c r="D118" s="28"/>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:4">
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
       <c r="D119" s="28"/>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:4">
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
       <c r="D120" s="28"/>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:4">
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
       <c r="D121" s="28"/>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:4">
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
       <c r="D122" s="28"/>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:4">
       <c r="B123" s="5"/>
       <c r="C123" s="5"/>
       <c r="D123" s="28"/>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:4">
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
       <c r="D124" s="28"/>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:4">
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
       <c r="D125" s="28"/>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:4">
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
       <c r="D126" s="28"/>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:4">
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
       <c r="D127" s="28"/>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:4">
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
       <c r="D128" s="28"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:4">
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
       <c r="D129" s="28"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:4">
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
       <c r="D130" s="28"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:4">
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
       <c r="D131" s="28"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:4">
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
       <c r="D132" s="28"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:4">
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
       <c r="D133" s="28"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:4">
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
       <c r="D134" s="28"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:4">
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
       <c r="D135" s="28"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:4">
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
       <c r="D136" s="28"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:4">
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
       <c r="D137" s="28"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:4">
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
       <c r="D138" s="28"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:4">
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
       <c r="D139" s="28"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:4">
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
       <c r="D140" s="28"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:4">
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
       <c r="D141" s="28"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:4">
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
       <c r="D142" s="28"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:4">
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
       <c r="D143" s="28"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:4">
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
       <c r="D144" s="28"/>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:4">
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
       <c r="D145" s="28"/>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:4">
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
       <c r="D146" s="28"/>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:4">
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
       <c r="D147" s="28"/>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:4">
       <c r="B148" s="5"/>
       <c r="C148" s="5"/>
       <c r="D148" s="28"/>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:4">
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
       <c r="D149" s="28"/>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:4">
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
       <c r="D150" s="28"/>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:4">
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
       <c r="D151" s="28"/>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:4">
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
       <c r="D152" s="28"/>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:4">
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
       <c r="D153" s="28"/>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:4">
       <c r="B154" s="5"/>
       <c r="C154" s="5"/>
       <c r="D154" s="28"/>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:4">
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
       <c r="D155" s="28"/>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:4">
       <c r="B156" s="5"/>
       <c r="C156" s="5"/>
       <c r="D156" s="28"/>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:4">
       <c r="B157" s="5"/>
       <c r="C157" s="5"/>
       <c r="D157" s="28"/>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:4">
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
       <c r="D158" s="28"/>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:4">
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
       <c r="D159" s="28"/>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:4">
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
       <c r="D160" s="28"/>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:4">
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
       <c r="D161" s="28"/>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:4">
       <c r="B162" s="5"/>
       <c r="C162" s="5"/>
       <c r="D162" s="28"/>
     </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:4">
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
       <c r="D163" s="28"/>
     </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:4">
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
       <c r="D164" s="28"/>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:4">
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
       <c r="D165" s="28"/>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:4">
       <c r="B166" s="5"/>
       <c r="C166" s="5"/>
       <c r="D166" s="28"/>
@@ -3151,42 +3243,47 @@
     <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A17:AM176"/>
+  <dimension ref="A17:AM180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="16" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="16" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="U133" sqref="U133"/>
+      <selection pane="bottomLeft" activeCell="AC178" sqref="AC178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="1.42578125" customWidth="1"/>
-    <col min="5" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="1.42578125" customWidth="1"/>
-    <col min="8" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="1.42578125" customWidth="1"/>
-    <col min="12" max="14" width="9.7109375" customWidth="1"/>
-    <col min="15" max="15" width="1.42578125" customWidth="1"/>
-    <col min="16" max="21" width="8.7109375" customWidth="1"/>
-    <col min="22" max="22" width="1.42578125" customWidth="1"/>
-    <col min="23" max="24" width="10.7109375" customWidth="1"/>
-    <col min="25" max="25" width="1.42578125" customWidth="1"/>
-    <col min="26" max="27" width="10.7109375" customWidth="1"/>
-    <col min="28" max="28" width="1.42578125" customWidth="1"/>
-    <col min="31" max="31" width="1.42578125" customWidth="1"/>
-    <col min="37" max="37" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="1.5" customWidth="1"/>
+    <col min="5" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="1.5" customWidth="1"/>
+    <col min="8" max="10" width="9.6640625" customWidth="1"/>
+    <col min="11" max="11" width="1.5" customWidth="1"/>
+    <col min="12" max="14" width="9.6640625" customWidth="1"/>
+    <col min="15" max="15" width="1.5" customWidth="1"/>
+    <col min="16" max="21" width="8.6640625" customWidth="1"/>
+    <col min="22" max="22" width="1.5" customWidth="1"/>
+    <col min="23" max="24" width="10.6640625" customWidth="1"/>
+    <col min="25" max="25" width="1.5" customWidth="1"/>
+    <col min="26" max="27" width="10.6640625" customWidth="1"/>
+    <col min="28" max="28" width="1.5" customWidth="1"/>
+    <col min="31" max="31" width="1.5" customWidth="1"/>
+    <col min="37" max="37" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="17" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" ht="15" thickBot="1">
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
@@ -3244,7 +3341,7 @@
       </c>
       <c r="AM17" s="57"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39">
       <c r="A18" s="13" t="s">
         <v>52</v>
       </c>
@@ -3339,7 +3436,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -3400,14 +3497,14 @@
         <v>203</v>
       </c>
       <c r="AD19" s="11">
-        <f>COUNTIF($N$19:$N$165, "&lt;0.41")</f>
+        <f>COUNTIF($N$19:$N$1000, "&lt;0.41")</f>
         <v>0</v>
       </c>
       <c r="AF19" s="43" t="s">
         <v>203</v>
       </c>
       <c r="AG19" s="44">
-        <f>COUNTIF($J$19:$J$165, "&lt;0.41")</f>
+        <f>COUNTIF($J$19:$J$1000, "&lt;0.41")</f>
         <v>0</v>
       </c>
       <c r="AI19" s="48">
@@ -3424,7 +3521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -3485,14 +3582,14 @@
         <v>0.41</v>
       </c>
       <c r="AD20" s="11">
-        <f>COUNTIF($N$19:$N$165, "&gt;="&amp;$AC20)-COUNTIF($N$19:$N$165,"&gt;="&amp;$AC21)</f>
+        <f>COUNTIF($N$19:$N$1000, "&gt;="&amp;$AC20)-COUNTIF($N$19:$N$1000,"&gt;="&amp;$AC21)</f>
         <v>1</v>
       </c>
       <c r="AF20" s="24">
         <v>0.41</v>
       </c>
       <c r="AG20" s="11">
-        <f>COUNTIF($J$19:$J$165, "&gt;="&amp;$AC20)-COUNTIF($J$19:$J$165,"&gt;="&amp;$AC21)</f>
+        <f>COUNTIF($J$19:$J$1000, "&gt;="&amp;$AC20)-COUNTIF($J$19:$J$1000,"&gt;="&amp;$AC21)</f>
         <v>0</v>
       </c>
       <c r="AI20" s="48">
@@ -3509,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -3570,14 +3667,14 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="AD21" s="11">
-        <f t="shared" ref="AD21:AD50" si="2">COUNTIF($N$19:$N$165, "&gt;="&amp;$AC21)-COUNTIF($N$19:$N$165,"&gt;="&amp;$AC22)</f>
+        <f t="shared" ref="AD21:AD52" si="2">COUNTIF($N$19:$N$1000, "&gt;="&amp;$AC21)-COUNTIF($N$19:$N$1000,"&gt;="&amp;$AC22)</f>
         <v>0</v>
       </c>
       <c r="AF21" s="24">
         <v>0.41499999999999998</v>
       </c>
       <c r="AG21" s="11">
-        <f t="shared" ref="AG21:AG50" si="3">COUNTIF($J$19:$J$165, "&gt;="&amp;$AC21)-COUNTIF($J$19:$J$165,"&gt;="&amp;$AC22)</f>
+        <f t="shared" ref="AG21:AG52" si="3">COUNTIF($J$19:$J$1000, "&gt;="&amp;$AC21)-COUNTIF($J$19:$J$1000,"&gt;="&amp;$AC22)</f>
         <v>0</v>
       </c>
       <c r="AI21" s="48">
@@ -3594,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -3656,7 +3753,7 @@
       </c>
       <c r="AD22" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF22" s="24">
         <v>0.42</v>
@@ -3679,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -3741,7 +3838,7 @@
       </c>
       <c r="AD23" s="11">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AF23" s="24">
         <v>0.42499999999999999</v>
@@ -3764,7 +3861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -3826,7 +3923,7 @@
       </c>
       <c r="AD24" s="11">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AF24" s="24">
         <v>0.43</v>
@@ -3849,7 +3946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -3911,7 +4008,7 @@
       </c>
       <c r="AD25" s="11">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="AF25" s="24">
         <v>0.435</v>
@@ -3934,7 +4031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -3996,7 +4093,7 @@
       </c>
       <c r="AD26" s="11">
         <f t="shared" si="2"/>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="AF26" s="24">
         <v>0.44</v>
@@ -4019,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -4081,7 +4178,7 @@
       </c>
       <c r="AD27" s="11">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AF27" s="24">
         <v>0.44500000000000001</v>
@@ -4104,7 +4201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -4189,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -4251,7 +4348,7 @@
       </c>
       <c r="AD29" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF29" s="24">
         <v>0.45500000000000002</v>
@@ -4274,7 +4371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -4359,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -4444,7 +4541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -4529,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -4614,7 +4711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -4699,7 +4796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -4784,7 +4881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -4869,7 +4966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -4954,7 +5051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39">
       <c r="A38" t="s">
         <v>56</v>
       </c>
@@ -5039,7 +5136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -5124,7 +5221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -5209,7 +5306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -5294,7 +5391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -5363,7 +5460,7 @@
       </c>
       <c r="AG42" s="11">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AI42" s="48">
         <v>0.54500000000000004</v>
@@ -5379,7 +5476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -5448,7 +5545,7 @@
       </c>
       <c r="AG43" s="11">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AI43" s="48">
         <v>0.55000000000000004</v>
@@ -5464,7 +5561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -5533,7 +5630,7 @@
       </c>
       <c r="AG44" s="11">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AI44" s="48">
         <v>0.55500000000000005</v>
@@ -5549,7 +5646,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -5618,7 +5715,7 @@
       </c>
       <c r="AG45" s="11">
         <f t="shared" si="3"/>
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="AI45" s="48">
         <v>0.56000000000000005</v>
@@ -5634,7 +5731,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -5703,7 +5800,7 @@
       </c>
       <c r="AG46" s="11">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AI46" s="48">
         <v>0.56499999999999995</v>
@@ -5719,7 +5816,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -5804,7 +5901,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -5889,7 +5986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:39">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -5974,7 +6071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:39">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -6058,7 +6155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:39" ht="15" thickBot="1">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -6118,14 +6215,14 @@
         <v>0.58499999999999996</v>
       </c>
       <c r="AD51" s="11">
-        <f>COUNTIF($N$19:$N$165, "&gt;="&amp;$AC51)-COUNTIF($N$19:$N$165,"&gt;=0.590")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF51" s="24">
         <v>0.58499999999999996</v>
       </c>
       <c r="AG51" s="11">
-        <f>COUNTIF($J$19:$J$165, "&gt;="&amp;$AC51)-COUNTIF($J$19:$J$165,"&gt;=0.590")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI51" s="50" t="s">
@@ -6142,7 +6239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:39" ht="15" thickBot="1">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -6202,18 +6299,18 @@
         <v>72</v>
       </c>
       <c r="AD52" s="11">
-        <f>COUNTIF($N$19:$N$165,"&gt;=0.590")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF52" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="AG52" s="25">
-        <f>COUNTIF($J$19:$J$165,"&gt;=0.590")</f>
+      <c r="AG52" s="11">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:39">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -6274,7 +6371,7 @@
       <c r="AF53" s="24"/>
       <c r="AG53" s="11"/>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -6353,7 +6450,7 @@
       <c r="AF54" s="24"/>
       <c r="AG54" s="11"/>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -6432,7 +6529,7 @@
       <c r="AF55" s="24"/>
       <c r="AG55" s="11"/>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -6511,7 +6608,7 @@
       <c r="AF56" s="24"/>
       <c r="AG56" s="11"/>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:39">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -6590,7 +6687,7 @@
       <c r="AF57" s="24"/>
       <c r="AG57" s="11"/>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:39">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -6669,7 +6766,7 @@
       <c r="AF58" s="24"/>
       <c r="AG58" s="11"/>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:39">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -6748,7 +6845,7 @@
       <c r="AF59" s="24"/>
       <c r="AG59" s="11"/>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:39">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -6827,7 +6924,7 @@
       <c r="AF60" s="24"/>
       <c r="AG60" s="11"/>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -6906,7 +7003,7 @@
       <c r="AF61" s="24"/>
       <c r="AG61" s="11"/>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -6985,7 +7082,7 @@
       <c r="AF62" s="24"/>
       <c r="AG62" s="11"/>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:39">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -7064,7 +7161,7 @@
       <c r="AF63" s="24"/>
       <c r="AG63" s="11"/>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:39">
       <c r="A64" t="s">
         <v>59</v>
       </c>
@@ -7143,7 +7240,7 @@
       <c r="AF64" s="24"/>
       <c r="AG64" s="11"/>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:33">
       <c r="A65" t="s">
         <v>59</v>
       </c>
@@ -7222,7 +7319,7 @@
       <c r="AF65" s="24"/>
       <c r="AG65" s="11"/>
     </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:33">
       <c r="A66" t="s">
         <v>59</v>
       </c>
@@ -7301,7 +7398,7 @@
       <c r="AF66" s="24"/>
       <c r="AG66" s="11"/>
     </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:33">
       <c r="A67" t="s">
         <v>59</v>
       </c>
@@ -7380,7 +7477,7 @@
       <c r="AF67" s="24"/>
       <c r="AG67" s="11"/>
     </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:33">
       <c r="A68" t="s">
         <v>59</v>
       </c>
@@ -7459,7 +7556,7 @@
       <c r="AF68" s="24"/>
       <c r="AG68" s="11"/>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:33">
       <c r="A69" t="s">
         <v>59</v>
       </c>
@@ -7538,7 +7635,7 @@
       <c r="AF69" s="24"/>
       <c r="AG69" s="11"/>
     </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:33">
       <c r="A70" t="s">
         <v>59</v>
       </c>
@@ -7617,7 +7714,7 @@
       <c r="AF70" s="24"/>
       <c r="AG70" s="11"/>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:33">
       <c r="A71" t="s">
         <v>59</v>
       </c>
@@ -7696,7 +7793,7 @@
       <c r="AF71" s="24"/>
       <c r="AG71" s="11"/>
     </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:33">
       <c r="A72" t="s">
         <v>59</v>
       </c>
@@ -7775,7 +7872,7 @@
       <c r="AF72" s="24"/>
       <c r="AG72" s="11"/>
     </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:33">
       <c r="A73" t="s">
         <v>59</v>
       </c>
@@ -7854,7 +7951,7 @@
       <c r="AF73" s="24"/>
       <c r="AG73" s="11"/>
     </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:33">
       <c r="A74" t="s">
         <v>59</v>
       </c>
@@ -7933,7 +8030,7 @@
       <c r="AF74" s="24"/>
       <c r="AG74" s="11"/>
     </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:33">
       <c r="A75" t="s">
         <v>59</v>
       </c>
@@ -8012,7 +8109,7 @@
       <c r="AF75" s="24"/>
       <c r="AG75" s="11"/>
     </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:33">
       <c r="A76" t="s">
         <v>59</v>
       </c>
@@ -8091,7 +8188,7 @@
       <c r="AF76" s="24"/>
       <c r="AG76" s="11"/>
     </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:33">
       <c r="A77" t="s">
         <v>59</v>
       </c>
@@ -8170,7 +8267,7 @@
       <c r="AF77" s="24"/>
       <c r="AG77" s="11"/>
     </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:33">
       <c r="A78" t="s">
         <v>59</v>
       </c>
@@ -8249,7 +8346,7 @@
       <c r="AF78" s="24"/>
       <c r="AG78" s="11"/>
     </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:33">
       <c r="A79" t="s">
         <v>59</v>
       </c>
@@ -8328,7 +8425,7 @@
       <c r="AF79" s="24"/>
       <c r="AG79" s="11"/>
     </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:33">
       <c r="A80" t="s">
         <v>59</v>
       </c>
@@ -8407,7 +8504,7 @@
       <c r="AF80" s="24"/>
       <c r="AG80" s="11"/>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:33">
       <c r="A81" t="s">
         <v>59</v>
       </c>
@@ -8486,7 +8583,7 @@
       <c r="AF81" s="24"/>
       <c r="AG81" s="11"/>
     </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:33">
       <c r="A82" t="s">
         <v>59</v>
       </c>
@@ -8565,7 +8662,7 @@
       <c r="AF82" s="24"/>
       <c r="AG82" s="11"/>
     </row>
-    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:33">
       <c r="A83" t="s">
         <v>59</v>
       </c>
@@ -8644,7 +8741,7 @@
       <c r="AF83" s="24"/>
       <c r="AG83" s="11"/>
     </row>
-    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:33">
       <c r="A84" t="s">
         <v>59</v>
       </c>
@@ -8723,7 +8820,7 @@
       <c r="AF84" s="24"/>
       <c r="AG84" s="11"/>
     </row>
-    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:33">
       <c r="A85" t="s">
         <v>59</v>
       </c>
@@ -8802,7 +8899,7 @@
       <c r="AF85" s="24"/>
       <c r="AG85" s="11"/>
     </row>
-    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:33">
       <c r="A86" t="s">
         <v>59</v>
       </c>
@@ -8881,7 +8978,7 @@
       <c r="AF86" s="24"/>
       <c r="AG86" s="11"/>
     </row>
-    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:33">
       <c r="A87" t="s">
         <v>59</v>
       </c>
@@ -8960,7 +9057,7 @@
       <c r="AF87" s="24"/>
       <c r="AG87" s="11"/>
     </row>
-    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:33">
       <c r="A88" t="s">
         <v>59</v>
       </c>
@@ -9039,7 +9136,7 @@
       <c r="AF88" s="24"/>
       <c r="AG88" s="11"/>
     </row>
-    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:33">
       <c r="A89" t="s">
         <v>59</v>
       </c>
@@ -9118,7 +9215,7 @@
       <c r="AF89" s="24"/>
       <c r="AG89" s="11"/>
     </row>
-    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:33">
       <c r="A90" t="s">
         <v>59</v>
       </c>
@@ -9197,7 +9294,7 @@
       <c r="AF90" s="24"/>
       <c r="AG90" s="11"/>
     </row>
-    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:33">
       <c r="A91" t="s">
         <v>59</v>
       </c>
@@ -9276,7 +9373,7 @@
       <c r="AF91" s="24"/>
       <c r="AG91" s="11"/>
     </row>
-    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:33">
       <c r="A92" t="s">
         <v>59</v>
       </c>
@@ -9355,7 +9452,7 @@
       <c r="AF92" s="24"/>
       <c r="AG92" s="11"/>
     </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:33">
       <c r="A93" t="s">
         <v>59</v>
       </c>
@@ -9434,7 +9531,7 @@
       <c r="AF93" s="24"/>
       <c r="AG93" s="11"/>
     </row>
-    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:33">
       <c r="A94" t="s">
         <v>59</v>
       </c>
@@ -9513,7 +9610,7 @@
       <c r="AF94" s="24"/>
       <c r="AG94" s="11"/>
     </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:33">
       <c r="A95" t="s">
         <v>59</v>
       </c>
@@ -9592,7 +9689,7 @@
       <c r="AF95" s="24"/>
       <c r="AG95" s="11"/>
     </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:33">
       <c r="A96" t="s">
         <v>59</v>
       </c>
@@ -9671,7 +9768,7 @@
       <c r="AF96" s="24"/>
       <c r="AG96" s="11"/>
     </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:33">
       <c r="A97" t="s">
         <v>59</v>
       </c>
@@ -9750,7 +9847,7 @@
       <c r="AF97" s="24"/>
       <c r="AG97" s="11"/>
     </row>
-    <row r="98" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:33">
       <c r="A98" t="s">
         <v>59</v>
       </c>
@@ -9820,7 +9917,7 @@
       <c r="AF98" s="24"/>
       <c r="AG98" s="11"/>
     </row>
-    <row r="99" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:33">
       <c r="A99" t="s">
         <v>59</v>
       </c>
@@ -9899,7 +9996,7 @@
       <c r="AF99" s="24"/>
       <c r="AG99" s="11"/>
     </row>
-    <row r="100" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:33">
       <c r="A100" t="s">
         <v>59</v>
       </c>
@@ -9978,7 +10075,7 @@
       <c r="AF100" s="24"/>
       <c r="AG100" s="11"/>
     </row>
-    <row r="101" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:33">
       <c r="A101" t="s">
         <v>59</v>
       </c>
@@ -10057,7 +10154,7 @@
       <c r="AF101" s="24"/>
       <c r="AG101" s="11"/>
     </row>
-    <row r="102" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:33">
       <c r="A102" t="s">
         <v>59</v>
       </c>
@@ -10136,7 +10233,7 @@
       <c r="AF102" s="24"/>
       <c r="AG102" s="11"/>
     </row>
-    <row r="103" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:33">
       <c r="A103" t="s">
         <v>59</v>
       </c>
@@ -10215,7 +10312,7 @@
       <c r="AF103" s="24"/>
       <c r="AG103" s="11"/>
     </row>
-    <row r="104" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:33">
       <c r="A104" t="s">
         <v>59</v>
       </c>
@@ -10294,7 +10391,7 @@
       <c r="AF104" s="24"/>
       <c r="AG104" s="11"/>
     </row>
-    <row r="105" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:33">
       <c r="A105" t="s">
         <v>59</v>
       </c>
@@ -10373,7 +10470,7 @@
       <c r="AF105" s="24"/>
       <c r="AG105" s="11"/>
     </row>
-    <row r="106" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:33">
       <c r="A106" t="s">
         <v>59</v>
       </c>
@@ -10452,7 +10549,7 @@
       <c r="AF106" s="24"/>
       <c r="AG106" s="11"/>
     </row>
-    <row r="107" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:33">
       <c r="A107" t="s">
         <v>59</v>
       </c>
@@ -10531,7 +10628,7 @@
       <c r="AF107" s="24"/>
       <c r="AG107" s="11"/>
     </row>
-    <row r="108" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:33">
       <c r="A108" t="s">
         <v>59</v>
       </c>
@@ -10610,7 +10707,7 @@
       <c r="AF108" s="24"/>
       <c r="AG108" s="11"/>
     </row>
-    <row r="109" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:33">
       <c r="A109" t="s">
         <v>59</v>
       </c>
@@ -10689,7 +10786,7 @@
       <c r="AF109" s="24"/>
       <c r="AG109" s="11"/>
     </row>
-    <row r="110" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:33">
       <c r="A110" t="s">
         <v>59</v>
       </c>
@@ -10768,7 +10865,7 @@
       <c r="AF110" s="24"/>
       <c r="AG110" s="11"/>
     </row>
-    <row r="111" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:33">
       <c r="A111" t="s">
         <v>59</v>
       </c>
@@ -10847,7 +10944,7 @@
       <c r="AF111" s="24"/>
       <c r="AG111" s="11"/>
     </row>
-    <row r="112" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:33">
       <c r="A112" t="s">
         <v>59</v>
       </c>
@@ -10926,7 +11023,7 @@
       <c r="AF112" s="24"/>
       <c r="AG112" s="11"/>
     </row>
-    <row r="113" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:33">
       <c r="A113" t="s">
         <v>59</v>
       </c>
@@ -11005,7 +11102,7 @@
       <c r="AF113" s="24"/>
       <c r="AG113" s="11"/>
     </row>
-    <row r="114" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:33">
       <c r="A114" t="s">
         <v>59</v>
       </c>
@@ -11084,7 +11181,7 @@
       <c r="AF114" s="24"/>
       <c r="AG114" s="11"/>
     </row>
-    <row r="115" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:33">
       <c r="A115" t="s">
         <v>59</v>
       </c>
@@ -11163,7 +11260,7 @@
       <c r="AF115" s="24"/>
       <c r="AG115" s="11"/>
     </row>
-    <row r="116" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:33">
       <c r="A116" t="s">
         <v>59</v>
       </c>
@@ -11242,7 +11339,7 @@
       <c r="AF116" s="24"/>
       <c r="AG116" s="11"/>
     </row>
-    <row r="117" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:33">
       <c r="A117" t="s">
         <v>59</v>
       </c>
@@ -11321,7 +11418,7 @@
       <c r="AF117" s="24"/>
       <c r="AG117" s="11"/>
     </row>
-    <row r="118" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:33">
       <c r="A118" t="s">
         <v>59</v>
       </c>
@@ -11400,7 +11497,7 @@
       <c r="AF118" s="24"/>
       <c r="AG118" s="11"/>
     </row>
-    <row r="119" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:33">
       <c r="A119" t="s">
         <v>59</v>
       </c>
@@ -11479,7 +11576,7 @@
       <c r="AF119" s="24"/>
       <c r="AG119" s="11"/>
     </row>
-    <row r="120" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:33">
       <c r="A120" t="s">
         <v>59</v>
       </c>
@@ -11558,7 +11655,7 @@
       <c r="AF120" s="24"/>
       <c r="AG120" s="11"/>
     </row>
-    <row r="121" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:33">
       <c r="A121" t="s">
         <v>59</v>
       </c>
@@ -11637,7 +11734,7 @@
       <c r="AF121" s="24"/>
       <c r="AG121" s="11"/>
     </row>
-    <row r="122" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:33">
       <c r="A122" t="s">
         <v>59</v>
       </c>
@@ -11716,7 +11813,7 @@
       <c r="AF122" s="24"/>
       <c r="AG122" s="11"/>
     </row>
-    <row r="123" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:33">
       <c r="A123" t="s">
         <v>59</v>
       </c>
@@ -11795,7 +11892,7 @@
       <c r="AF123" s="24"/>
       <c r="AG123" s="11"/>
     </row>
-    <row r="124" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:33">
       <c r="A124" t="s">
         <v>59</v>
       </c>
@@ -11874,7 +11971,7 @@
       <c r="AF124" s="24"/>
       <c r="AG124" s="11"/>
     </row>
-    <row r="125" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:33">
       <c r="A125" t="s">
         <v>59</v>
       </c>
@@ -11953,7 +12050,7 @@
       <c r="AF125" s="24"/>
       <c r="AG125" s="11"/>
     </row>
-    <row r="126" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:33">
       <c r="A126" t="s">
         <v>59</v>
       </c>
@@ -12032,7 +12129,7 @@
       <c r="AF126" s="24"/>
       <c r="AG126" s="11"/>
     </row>
-    <row r="127" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:33">
       <c r="A127" t="s">
         <v>59</v>
       </c>
@@ -12111,7 +12208,7 @@
       <c r="AF127" s="24"/>
       <c r="AG127" s="11"/>
     </row>
-    <row r="128" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:33">
       <c r="A128" t="s">
         <v>59</v>
       </c>
@@ -12190,7 +12287,7 @@
       <c r="AF128" s="24"/>
       <c r="AG128" s="11"/>
     </row>
-    <row r="129" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:33">
       <c r="A129" t="s">
         <v>59</v>
       </c>
@@ -12269,7 +12366,7 @@
       <c r="AF129" s="24"/>
       <c r="AG129" s="11"/>
     </row>
-    <row r="130" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:33">
       <c r="A130" t="s">
         <v>59</v>
       </c>
@@ -12348,7 +12445,7 @@
       <c r="AF130" s="24"/>
       <c r="AG130" s="11"/>
     </row>
-    <row r="131" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:33">
       <c r="A131" t="s">
         <v>59</v>
       </c>
@@ -12427,7 +12524,7 @@
       <c r="AF131" s="24"/>
       <c r="AG131" s="11"/>
     </row>
-    <row r="132" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:33">
       <c r="A132" t="s">
         <v>170</v>
       </c>
@@ -12497,7 +12594,7 @@
       <c r="AF132" s="24"/>
       <c r="AG132" s="11"/>
     </row>
-    <row r="133" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:33">
       <c r="A133" t="s">
         <v>170</v>
       </c>
@@ -12567,7 +12664,7 @@
       <c r="AF133" s="24"/>
       <c r="AG133" s="11"/>
     </row>
-    <row r="134" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:33">
       <c r="A134" t="s">
         <v>173</v>
       </c>
@@ -12643,7 +12740,7 @@
       <c r="AF134" s="24"/>
       <c r="AG134" s="11"/>
     </row>
-    <row r="135" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:33">
       <c r="A135" t="s">
         <v>173</v>
       </c>
@@ -12719,7 +12816,7 @@
       <c r="AF135" s="24"/>
       <c r="AG135" s="11"/>
     </row>
-    <row r="136" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:33">
       <c r="A136" t="s">
         <v>173</v>
       </c>
@@ -12795,7 +12892,7 @@
       <c r="AF136" s="24"/>
       <c r="AG136" s="11"/>
     </row>
-    <row r="137" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:33">
       <c r="A137" t="s">
         <v>173</v>
       </c>
@@ -12871,7 +12968,7 @@
       <c r="AF137" s="24"/>
       <c r="AG137" s="11"/>
     </row>
-    <row r="138" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:33">
       <c r="A138" t="s">
         <v>173</v>
       </c>
@@ -12947,7 +13044,7 @@
       <c r="AF138" s="24"/>
       <c r="AG138" s="11"/>
     </row>
-    <row r="139" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:33">
       <c r="A139" t="s">
         <v>173</v>
       </c>
@@ -13023,7 +13120,7 @@
       <c r="AF139" s="24"/>
       <c r="AG139" s="11"/>
     </row>
-    <row r="140" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:33">
       <c r="A140" t="s">
         <v>173</v>
       </c>
@@ -13099,7 +13196,7 @@
       <c r="AF140" s="24"/>
       <c r="AG140" s="11"/>
     </row>
-    <row r="141" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:33">
       <c r="A141" t="s">
         <v>173</v>
       </c>
@@ -13175,7 +13272,7 @@
       <c r="AF141" s="24"/>
       <c r="AG141" s="11"/>
     </row>
-    <row r="142" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:33">
       <c r="A142" t="s">
         <v>173</v>
       </c>
@@ -13251,7 +13348,7 @@
       <c r="AF142" s="24"/>
       <c r="AG142" s="11"/>
     </row>
-    <row r="143" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:33">
       <c r="A143" t="s">
         <v>173</v>
       </c>
@@ -13327,7 +13424,7 @@
       <c r="AF143" s="24"/>
       <c r="AG143" s="11"/>
     </row>
-    <row r="144" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:33">
       <c r="A144" t="s">
         <v>173</v>
       </c>
@@ -13403,7 +13500,7 @@
       <c r="AF144" s="24"/>
       <c r="AG144" s="11"/>
     </row>
-    <row r="145" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:33">
       <c r="A145" t="s">
         <v>173</v>
       </c>
@@ -13479,7 +13576,7 @@
       <c r="AF145" s="24"/>
       <c r="AG145" s="11"/>
     </row>
-    <row r="146" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:33">
       <c r="A146" t="s">
         <v>173</v>
       </c>
@@ -13555,7 +13652,7 @@
       <c r="AF146" s="24"/>
       <c r="AG146" s="11"/>
     </row>
-    <row r="147" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:33">
       <c r="A147" t="s">
         <v>173</v>
       </c>
@@ -13631,7 +13728,7 @@
       <c r="AF147" s="24"/>
       <c r="AG147" s="11"/>
     </row>
-    <row r="148" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:33">
       <c r="A148" t="s">
         <v>173</v>
       </c>
@@ -13707,7 +13804,7 @@
       <c r="AF148" s="24"/>
       <c r="AG148" s="11"/>
     </row>
-    <row r="149" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:33">
       <c r="A149" t="s">
         <v>173</v>
       </c>
@@ -13783,7 +13880,7 @@
       <c r="AF149" s="24"/>
       <c r="AG149" s="11"/>
     </row>
-    <row r="150" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:33">
       <c r="A150" t="s">
         <v>173</v>
       </c>
@@ -13859,7 +13956,7 @@
       <c r="AF150" s="24"/>
       <c r="AG150" s="11"/>
     </row>
-    <row r="151" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:33">
       <c r="A151" t="s">
         <v>173</v>
       </c>
@@ -13935,7 +14032,7 @@
       <c r="AF151" s="24"/>
       <c r="AG151" s="11"/>
     </row>
-    <row r="152" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:33">
       <c r="A152" t="s">
         <v>173</v>
       </c>
@@ -14011,7 +14108,7 @@
       <c r="AF152" s="24"/>
       <c r="AG152" s="11"/>
     </row>
-    <row r="153" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:33">
       <c r="A153" t="s">
         <v>173</v>
       </c>
@@ -14087,7 +14184,7 @@
       <c r="AF153" s="24"/>
       <c r="AG153" s="11"/>
     </row>
-    <row r="154" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:33">
       <c r="A154" t="s">
         <v>173</v>
       </c>
@@ -14163,7 +14260,7 @@
       <c r="AF154" s="24"/>
       <c r="AG154" s="11"/>
     </row>
-    <row r="155" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:33">
       <c r="A155" t="s">
         <v>173</v>
       </c>
@@ -14239,7 +14336,7 @@
       <c r="AF155" s="24"/>
       <c r="AG155" s="11"/>
     </row>
-    <row r="156" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:33">
       <c r="A156" t="s">
         <v>173</v>
       </c>
@@ -14315,7 +14412,7 @@
       <c r="AF156" s="24"/>
       <c r="AG156" s="11"/>
     </row>
-    <row r="157" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:33">
       <c r="A157" t="s">
         <v>173</v>
       </c>
@@ -14391,7 +14488,7 @@
       <c r="AF157" s="24"/>
       <c r="AG157" s="11"/>
     </row>
-    <row r="158" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:33">
       <c r="A158" t="s">
         <v>173</v>
       </c>
@@ -14467,7 +14564,7 @@
       <c r="AF158" s="24"/>
       <c r="AG158" s="11"/>
     </row>
-    <row r="159" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:33">
       <c r="A159" t="s">
         <v>173</v>
       </c>
@@ -14543,7 +14640,7 @@
       <c r="AF159" s="24"/>
       <c r="AG159" s="11"/>
     </row>
-    <row r="160" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:33">
       <c r="A160" t="s">
         <v>173</v>
       </c>
@@ -14619,7 +14716,7 @@
       <c r="AF160" s="24"/>
       <c r="AG160" s="11"/>
     </row>
-    <row r="161" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:35">
       <c r="A161" t="s">
         <v>173</v>
       </c>
@@ -14695,7 +14792,7 @@
       <c r="AF161" s="24"/>
       <c r="AG161" s="11"/>
     </row>
-    <row r="162" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:35">
       <c r="A162" t="s">
         <v>173</v>
       </c>
@@ -14771,7 +14868,7 @@
       <c r="AF162" s="24"/>
       <c r="AG162" s="11"/>
     </row>
-    <row r="163" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:35">
       <c r="A163" t="s">
         <v>173</v>
       </c>
@@ -14847,7 +14944,7 @@
       <c r="AF163" s="24"/>
       <c r="AG163" s="11"/>
     </row>
-    <row r="164" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:35">
       <c r="A164" t="s">
         <v>173</v>
       </c>
@@ -14923,7 +15020,7 @@
       <c r="AF164" s="24"/>
       <c r="AG164" s="11"/>
     </row>
-    <row r="165" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:35">
       <c r="A165" t="s">
         <v>173</v>
       </c>
@@ -14999,25 +15096,305 @@
       <c r="AF165" s="24"/>
       <c r="AG165" s="11"/>
     </row>
-    <row r="166" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:35">
+      <c r="A166" t="s">
+        <v>204</v>
+      </c>
+      <c r="C166" t="s">
+        <v>205</v>
+      </c>
+      <c r="E166" s="41">
+        <v>3</v>
+      </c>
+      <c r="F166" t="s">
+        <v>65</v>
+      </c>
+      <c r="H166">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="I166">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="J166">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="L166">
+        <v>0.43</v>
+      </c>
+      <c r="M166">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="N166">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="P166" t="str">
+        <f>IF(AND(J166&lt;=Constants!F$5,J166&gt;=Constants!E$5),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="Q166" t="str">
+        <f>IF(AND(J166&lt;=Constants!F$6,J166&gt;=Constants!E$6),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="R166" t="str">
+        <f>IF(AND(J166&lt;=Constants!F$7,J166&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S166" t="str">
+        <f>IF(P166="N","N",IF(OR((J166+Constants!D$14)&gt;Constants!F$5,(J166-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="T166" t="str">
+        <f>IF(Q166="N","N",IF(OR((J166+Constants!D$14)&gt;Constants!F$6,(J166-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="U166" t="str">
+        <f>IF(R166="N","N",IF(OR((J166+Constants!D$14)&gt;Constants!F$7,(J166-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W166">
+        <f>J166/2+Constants!D$9-Constants!D$10</f>
+        <v>0.37</v>
+      </c>
+      <c r="X166">
+        <f>H166/2+Constants!D$9-Constants!D$11</f>
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="Z166">
+        <f t="shared" ref="Z166:Z180" si="8">1000*(W166-0.29)</f>
+        <v>80.000000000000014</v>
+      </c>
+      <c r="AA166">
+        <f t="shared" ref="AA166:AA180" si="9">1000*(X166-0.29)</f>
+        <v>57.999999999999993</v>
+      </c>
       <c r="AC166" s="24"/>
       <c r="AD166" s="11"/>
       <c r="AF166" s="24"/>
       <c r="AG166" s="11"/>
     </row>
-    <row r="167" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:35">
+      <c r="A167" t="s">
+        <v>219</v>
+      </c>
+      <c r="C167" t="s">
+        <v>206</v>
+      </c>
+      <c r="E167" s="41">
+        <v>2</v>
+      </c>
+      <c r="F167" t="s">
+        <v>65</v>
+      </c>
+      <c r="H167">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I167">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="J167">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="L167">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="M167">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="N167">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="P167" t="str">
+        <f>IF(AND(J167&lt;=Constants!F$5,J167&gt;=Constants!E$5),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="Q167" t="str">
+        <f>IF(AND(J167&lt;=Constants!F$6,J167&gt;=Constants!E$6),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="R167" t="str">
+        <f>IF(AND(J167&lt;=Constants!F$7,J167&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S167" t="str">
+        <f>IF(P167="N","N",IF(OR((J167+Constants!D$14)&gt;Constants!F$5,(J167-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="T167" t="str">
+        <f>IF(Q167="N","N",IF(OR((J167+Constants!D$14)&gt;Constants!F$6,(J167-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="U167" t="str">
+        <f>IF(R167="N","N",IF(OR((J167+Constants!D$14)&gt;Constants!F$7,(J167-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W167">
+        <f>J167/2+Constants!D$9-Constants!D$10</f>
+        <v>0.372</v>
+      </c>
+      <c r="X167">
+        <f>H167/2+Constants!D$9-Constants!D$11</f>
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="Z167">
+        <f t="shared" si="8"/>
+        <v>82.000000000000014</v>
+      </c>
+      <c r="AA167">
+        <f t="shared" si="9"/>
+        <v>61</v>
+      </c>
       <c r="AC167" s="24"/>
       <c r="AD167" s="11"/>
       <c r="AF167" s="24"/>
       <c r="AG167" s="11"/>
     </row>
-    <row r="168" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:35">
+      <c r="A168" t="s">
+        <v>220</v>
+      </c>
+      <c r="C168" t="s">
+        <v>207</v>
+      </c>
+      <c r="E168" s="41">
+        <v>3</v>
+      </c>
+      <c r="F168" t="s">
+        <v>65</v>
+      </c>
+      <c r="H168">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="I168">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="J168">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="L168">
+        <v>0.439</v>
+      </c>
+      <c r="M168">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="N168">
+        <v>0.439</v>
+      </c>
+      <c r="P168" t="str">
+        <f>IF(AND(J168&lt;=Constants!F$5,J168&gt;=Constants!E$5),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="Q168" t="str">
+        <f>IF(AND(J168&lt;=Constants!F$6,J168&gt;=Constants!E$6),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R168" t="str">
+        <f>IF(AND(J168&lt;=Constants!F$7,J168&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S168" t="str">
+        <f>IF(P168="N","N",IF(OR((J168+Constants!D$14)&gt;Constants!F$5,(J168-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="T168" t="str">
+        <f>IF(Q168="N","N",IF(OR((J168+Constants!D$14)&gt;Constants!F$6,(J168-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>Y</v>
+      </c>
+      <c r="U168" t="str">
+        <f>IF(R168="N","N",IF(OR((J168+Constants!D$14)&gt;Constants!F$7,(J168-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W168">
+        <f>J168/2+Constants!D$9-Constants!D$10</f>
+        <v>0.37350000000000005</v>
+      </c>
+      <c r="X168">
+        <f>H168/2+Constants!D$9-Constants!D$11</f>
+        <v>0.35150000000000003</v>
+      </c>
+      <c r="Z168">
+        <f t="shared" si="8"/>
+        <v>83.500000000000071</v>
+      </c>
+      <c r="AA168">
+        <f t="shared" si="9"/>
+        <v>61.500000000000057</v>
+      </c>
       <c r="AC168" s="24"/>
       <c r="AD168" s="11"/>
       <c r="AF168" s="24"/>
       <c r="AG168" s="11"/>
     </row>
-    <row r="169" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:35">
+      <c r="A169" t="s">
+        <v>221</v>
+      </c>
+      <c r="C169" t="s">
+        <v>208</v>
+      </c>
+      <c r="E169" s="41">
+        <v>3</v>
+      </c>
+      <c r="F169" t="s">
+        <v>65</v>
+      </c>
+      <c r="H169">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="I169">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="J169">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="L169">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="M169">
+        <v>0.439</v>
+      </c>
+      <c r="N169">
+        <v>0.439</v>
+      </c>
+      <c r="P169" t="str">
+        <f>IF(AND(J169&lt;=Constants!F$5,J169&gt;=Constants!E$5),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="Q169" t="str">
+        <f>IF(AND(J169&lt;=Constants!F$6,J169&gt;=Constants!E$6),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R169" t="str">
+        <f>IF(AND(J169&lt;=Constants!F$7,J169&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S169" t="str">
+        <f>IF(P169="N","N",IF(OR((J169+Constants!D$14)&gt;Constants!F$5,(J169-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="T169" t="str">
+        <f>IF(Q169="N","N",IF(OR((J169+Constants!D$14)&gt;Constants!F$6,(J169-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="U169" t="str">
+        <f>IF(R169="N","N",IF(OR((J169+Constants!D$14)&gt;Constants!F$7,(J169-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W169">
+        <f>J169/2+Constants!D$9-Constants!D$10</f>
+        <v>0.376</v>
+      </c>
+      <c r="X169">
+        <f>H169/2+Constants!D$9-Constants!D$11</f>
+        <v>0.35450000000000004</v>
+      </c>
+      <c r="Z169">
+        <f t="shared" si="8"/>
+        <v>86.000000000000014</v>
+      </c>
+      <c r="AA169">
+        <f t="shared" si="9"/>
+        <v>64.500000000000057</v>
+      </c>
       <c r="AC169" s="24"/>
       <c r="AD169" s="11"/>
       <c r="AE169" s="5"/>
@@ -15026,7 +15403,77 @@
       <c r="AH169" s="5"/>
       <c r="AI169" s="5"/>
     </row>
-    <row r="170" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:35">
+      <c r="A170" t="s">
+        <v>222</v>
+      </c>
+      <c r="C170" t="s">
+        <v>209</v>
+      </c>
+      <c r="E170" s="41">
+        <v>2</v>
+      </c>
+      <c r="F170" t="s">
+        <v>65</v>
+      </c>
+      <c r="H170">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="I170">
+        <v>0.55230000000000001</v>
+      </c>
+      <c r="J170">
+        <v>0.55230000000000001</v>
+      </c>
+      <c r="L170">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="M170">
+        <v>0.441</v>
+      </c>
+      <c r="N170">
+        <v>0.441</v>
+      </c>
+      <c r="P170" t="str">
+        <f>IF(AND(J170&lt;=Constants!F$5,J170&gt;=Constants!E$5),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="Q170" t="str">
+        <f>IF(AND(J170&lt;=Constants!F$6,J170&gt;=Constants!E$6),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R170" t="str">
+        <f>IF(AND(J170&lt;=Constants!F$7,J170&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S170" t="str">
+        <f>IF(P170="N","N",IF(OR((J170+Constants!D$14)&gt;Constants!F$5,(J170-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="T170" t="str">
+        <f>IF(Q170="N","N",IF(OR((J170+Constants!D$14)&gt;Constants!F$6,(J170-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>Y</v>
+      </c>
+      <c r="U170" t="str">
+        <f>IF(R170="N","N",IF(OR((J170+Constants!D$14)&gt;Constants!F$7,(J170-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W170">
+        <f>J170/2+Constants!D$9-Constants!D$10</f>
+        <v>0.37414999999999998</v>
+      </c>
+      <c r="X170">
+        <f>H170/2+Constants!D$9-Constants!D$11</f>
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="Z170">
+        <f t="shared" si="8"/>
+        <v>84.15</v>
+      </c>
+      <c r="AA170">
+        <f t="shared" si="9"/>
+        <v>68</v>
+      </c>
       <c r="AC170" s="24"/>
       <c r="AD170" s="11"/>
       <c r="AE170" s="5"/>
@@ -15035,7 +15482,77 @@
       <c r="AH170" s="5"/>
       <c r="AI170" s="5"/>
     </row>
-    <row r="171" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:35">
+      <c r="A171" t="s">
+        <v>223</v>
+      </c>
+      <c r="C171" t="s">
+        <v>210</v>
+      </c>
+      <c r="E171" s="41">
+        <v>3</v>
+      </c>
+      <c r="F171" t="s">
+        <v>65</v>
+      </c>
+      <c r="H171">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="I171">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="J171">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="L171">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="M171">
+        <v>0.439</v>
+      </c>
+      <c r="N171">
+        <v>0.439</v>
+      </c>
+      <c r="P171" t="str">
+        <f>IF(AND(J171&lt;=Constants!F$5,J171&gt;=Constants!E$5),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="Q171" t="str">
+        <f>IF(AND(J171&lt;=Constants!F$6,J171&gt;=Constants!E$6),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R171" t="str">
+        <f>IF(AND(J171&lt;=Constants!F$7,J171&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S171" t="str">
+        <f>IF(P171="N","N",IF(OR((J171+Constants!D$14)&gt;Constants!F$5,(J171-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="T171" t="str">
+        <f>IF(Q171="N","N",IF(OR((J171+Constants!D$14)&gt;Constants!F$6,(J171-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="U171" t="str">
+        <f>IF(R171="N","N",IF(OR((J171+Constants!D$14)&gt;Constants!F$7,(J171-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W171">
+        <f>J171/2+Constants!D$9-Constants!D$10</f>
+        <v>0.37650000000000006</v>
+      </c>
+      <c r="X171">
+        <f>H171/2+Constants!D$9-Constants!D$11</f>
+        <v>0.35650000000000004</v>
+      </c>
+      <c r="Z171">
+        <f t="shared" si="8"/>
+        <v>86.500000000000071</v>
+      </c>
+      <c r="AA171">
+        <f t="shared" si="9"/>
+        <v>66.500000000000057</v>
+      </c>
       <c r="AC171" s="24"/>
       <c r="AD171" s="11"/>
       <c r="AE171" s="5"/>
@@ -15044,7 +15561,77 @@
       <c r="AH171" s="5"/>
       <c r="AI171" s="5"/>
     </row>
-    <row r="172" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:35">
+      <c r="A172" t="s">
+        <v>224</v>
+      </c>
+      <c r="C172" t="s">
+        <v>211</v>
+      </c>
+      <c r="E172" s="41">
+        <v>2</v>
+      </c>
+      <c r="F172" t="s">
+        <v>65</v>
+      </c>
+      <c r="H172">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I172">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="J172">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="L172">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="M172">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="N172">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="P172" t="str">
+        <f>IF(AND(J172&lt;=Constants!F$5,J172&gt;=Constants!E$5),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="Q172" t="str">
+        <f>IF(AND(J172&lt;=Constants!F$6,J172&gt;=Constants!E$6),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R172" t="str">
+        <f>IF(AND(J172&lt;=Constants!F$7,J172&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S172" t="str">
+        <f>IF(P172="N","N",IF(OR((J172+Constants!D$14)&gt;Constants!F$5,(J172-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>Y</v>
+      </c>
+      <c r="T172" t="str">
+        <f>IF(Q172="N","N",IF(OR((J172+Constants!D$14)&gt;Constants!F$6,(J172-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="U172" t="str">
+        <f>IF(R172="N","N",IF(OR((J172+Constants!D$14)&gt;Constants!F$7,(J172-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W172">
+        <f>J172/2+Constants!D$9-Constants!D$10</f>
+        <v>0.379</v>
+      </c>
+      <c r="X172">
+        <f>H172/2+Constants!D$9-Constants!D$11</f>
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="Z172">
+        <f t="shared" si="8"/>
+        <v>89.000000000000028</v>
+      </c>
+      <c r="AA172">
+        <f t="shared" si="9"/>
+        <v>71.000000000000014</v>
+      </c>
       <c r="AC172" s="11"/>
       <c r="AD172" s="11"/>
       <c r="AE172" s="5"/>
@@ -15053,7 +15640,77 @@
       <c r="AH172" s="5"/>
       <c r="AI172" s="5"/>
     </row>
-    <row r="173" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:35">
+      <c r="A173" t="s">
+        <v>225</v>
+      </c>
+      <c r="C173" t="s">
+        <v>212</v>
+      </c>
+      <c r="E173" s="41">
+        <v>2</v>
+      </c>
+      <c r="F173" t="s">
+        <v>95</v>
+      </c>
+      <c r="H173">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I173">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J173">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L173">
+        <v>0.441</v>
+      </c>
+      <c r="M173">
+        <v>0.44</v>
+      </c>
+      <c r="N173">
+        <v>0.441</v>
+      </c>
+      <c r="P173" t="str">
+        <f>IF(AND(J173&lt;=Constants!F$5,J173&gt;=Constants!E$5),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="Q173" t="str">
+        <f>IF(AND(J173&lt;=Constants!F$6,J173&gt;=Constants!E$6),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R173" t="str">
+        <f>IF(AND(J173&lt;=Constants!F$7,J173&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S173" t="str">
+        <f>IF(P173="N","N",IF(OR((J173+Constants!D$14)&gt;Constants!F$5,(J173-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="T173" t="str">
+        <f>IF(Q173="N","N",IF(OR((J173+Constants!D$14)&gt;Constants!F$6,(J173-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>Y</v>
+      </c>
+      <c r="U173" t="str">
+        <f>IF(R173="N","N",IF(OR((J173+Constants!D$14)&gt;Constants!F$7,(J173-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W173">
+        <f>J173/2+Constants!D$9-Constants!D$10</f>
+        <v>0.373</v>
+      </c>
+      <c r="X173">
+        <f>H173/2+Constants!D$9-Constants!D$11</f>
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="Z173">
+        <f t="shared" si="8"/>
+        <v>83.000000000000014</v>
+      </c>
+      <c r="AA173">
+        <f t="shared" si="9"/>
+        <v>61</v>
+      </c>
       <c r="AC173" s="5"/>
       <c r="AD173" s="5"/>
       <c r="AE173" s="5"/>
@@ -15062,7 +15719,77 @@
       <c r="AH173" s="5"/>
       <c r="AI173" s="5"/>
     </row>
-    <row r="174" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:35">
+      <c r="A174" t="s">
+        <v>226</v>
+      </c>
+      <c r="C174" t="s">
+        <v>213</v>
+      </c>
+      <c r="E174" s="41">
+        <v>2</v>
+      </c>
+      <c r="F174" t="s">
+        <v>95</v>
+      </c>
+      <c r="H174">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="I174">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="J174">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="L174">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="M174">
+        <v>0.437</v>
+      </c>
+      <c r="N174">
+        <v>0.437</v>
+      </c>
+      <c r="P174" t="str">
+        <f>IF(AND(J174&lt;=Constants!F$5,J174&gt;=Constants!E$5),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="Q174" t="str">
+        <f>IF(AND(J174&lt;=Constants!F$6,J174&gt;=Constants!E$6),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R174" t="str">
+        <f>IF(AND(J174&lt;=Constants!F$7,J174&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S174" t="str">
+        <f>IF(P174="N","N",IF(OR((J174+Constants!D$14)&gt;Constants!F$5,(J174-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="T174" t="str">
+        <f>IF(Q174="N","N",IF(OR((J174+Constants!D$14)&gt;Constants!F$6,(J174-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="U174" t="str">
+        <f>IF(R174="N","N",IF(OR((J174+Constants!D$14)&gt;Constants!F$7,(J174-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W174">
+        <f>J174/2+Constants!D$9-Constants!D$10</f>
+        <v>0.37550000000000006</v>
+      </c>
+      <c r="X174">
+        <f>H174/2+Constants!D$9-Constants!D$11</f>
+        <v>0.35550000000000004</v>
+      </c>
+      <c r="Z174">
+        <f t="shared" si="8"/>
+        <v>85.500000000000071</v>
+      </c>
+      <c r="AA174">
+        <f t="shared" si="9"/>
+        <v>65.500000000000057</v>
+      </c>
       <c r="AC174" s="5"/>
       <c r="AD174" s="5"/>
       <c r="AE174" s="5"/>
@@ -15071,7 +15798,77 @@
       <c r="AH174" s="5"/>
       <c r="AI174" s="5"/>
     </row>
-    <row r="175" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:35">
+      <c r="A175" t="s">
+        <v>227</v>
+      </c>
+      <c r="C175" t="s">
+        <v>214</v>
+      </c>
+      <c r="E175" s="41">
+        <v>2</v>
+      </c>
+      <c r="F175" t="s">
+        <v>95</v>
+      </c>
+      <c r="H175">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="I175">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="J175">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="L175">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="M175">
+        <v>0.438</v>
+      </c>
+      <c r="N175">
+        <v>0.438</v>
+      </c>
+      <c r="P175" t="str">
+        <f>IF(AND(J175&lt;=Constants!F$5,J175&gt;=Constants!E$5),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="Q175" t="str">
+        <f>IF(AND(J175&lt;=Constants!F$6,J175&gt;=Constants!E$6),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R175" t="str">
+        <f>IF(AND(J175&lt;=Constants!F$7,J175&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S175" t="str">
+        <f>IF(P175="N","N",IF(OR((J175+Constants!D$14)&gt;Constants!F$5,(J175-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="T175" t="str">
+        <f>IF(Q175="N","N",IF(OR((J175+Constants!D$14)&gt;Constants!F$6,(J175-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>Y</v>
+      </c>
+      <c r="U175" t="str">
+        <f>IF(R175="N","N",IF(OR((J175+Constants!D$14)&gt;Constants!F$7,(J175-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W175">
+        <f>J175/2+Constants!D$9-Constants!D$10</f>
+        <v>0.375</v>
+      </c>
+      <c r="X175">
+        <f>H175/2+Constants!D$9-Constants!D$11</f>
+        <v>0.35450000000000004</v>
+      </c>
+      <c r="Z175">
+        <f t="shared" si="8"/>
+        <v>85.000000000000014</v>
+      </c>
+      <c r="AA175">
+        <f t="shared" si="9"/>
+        <v>64.500000000000057</v>
+      </c>
       <c r="AC175" s="5"/>
       <c r="AD175" s="5"/>
       <c r="AE175" s="5"/>
@@ -15080,11 +15877,369 @@
       <c r="AH175" s="5"/>
       <c r="AI175" s="5"/>
     </row>
-    <row r="176" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:35">
+      <c r="A176" t="s">
+        <v>228</v>
+      </c>
+      <c r="C176" t="s">
+        <v>215</v>
+      </c>
+      <c r="E176" s="41">
+        <v>2</v>
+      </c>
+      <c r="F176" t="s">
+        <v>95</v>
+      </c>
+      <c r="H176">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="I176">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="J176">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="L176">
+        <v>0.443</v>
+      </c>
+      <c r="M176">
+        <v>0.438</v>
+      </c>
+      <c r="N176">
+        <v>0.438</v>
+      </c>
+      <c r="P176" t="str">
+        <f>IF(AND(J176&lt;=Constants!F$5,J176&gt;=Constants!E$5),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="Q176" t="str">
+        <f>IF(AND(J176&lt;=Constants!F$6,J176&gt;=Constants!E$6),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R176" t="str">
+        <f>IF(AND(J176&lt;=Constants!F$7,J176&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S176" t="str">
+        <f>IF(P176="N","N",IF(OR((J176+Constants!D$14)&gt;Constants!F$5,(J176-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="T176" t="str">
+        <f>IF(Q176="N","N",IF(OR((J176+Constants!D$14)&gt;Constants!F$6,(J176-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>Y</v>
+      </c>
+      <c r="U176" t="str">
+        <f>IF(R176="N","N",IF(OR((J176+Constants!D$14)&gt;Constants!F$7,(J176-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W176">
+        <f>J176/2+Constants!D$9-Constants!D$10</f>
+        <v>0.37450000000000006</v>
+      </c>
+      <c r="X176">
+        <f>H176/2+Constants!D$9-Constants!D$11</f>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="Z176">
+        <f t="shared" si="8"/>
+        <v>84.500000000000071</v>
+      </c>
+      <c r="AA176">
+        <f t="shared" si="9"/>
+        <v>65</v>
+      </c>
       <c r="AC176" s="5"/>
       <c r="AD176" s="5"/>
       <c r="AF176" s="5"/>
       <c r="AG176" s="5"/>
+    </row>
+    <row r="177" spans="1:27">
+      <c r="A177" t="s">
+        <v>229</v>
+      </c>
+      <c r="C177" t="s">
+        <v>215</v>
+      </c>
+      <c r="E177" s="41">
+        <v>2</v>
+      </c>
+      <c r="F177" t="s">
+        <v>95</v>
+      </c>
+      <c r="H177">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I177">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="J177">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L177">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="M177">
+        <v>0.43</v>
+      </c>
+      <c r="N177">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="P177" t="str">
+        <f>IF(AND(J177&lt;=Constants!F$5,J177&gt;=Constants!E$5),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="Q177" t="str">
+        <f>IF(AND(J177&lt;=Constants!F$6,J177&gt;=Constants!E$6),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R177" t="str">
+        <f>IF(AND(J177&lt;=Constants!F$7,J177&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S177" t="str">
+        <f>IF(P177="N","N",IF(OR((J177+Constants!D$14)&gt;Constants!F$5,(J177-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="T177" t="str">
+        <f>IF(Q177="N","N",IF(OR((J177+Constants!D$14)&gt;Constants!F$6,(J177-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>Y</v>
+      </c>
+      <c r="U177" t="str">
+        <f>IF(R177="N","N",IF(OR((J177+Constants!D$14)&gt;Constants!F$7,(J177-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W177">
+        <f>J177/2+Constants!D$9-Constants!D$10</f>
+        <v>0.373</v>
+      </c>
+      <c r="X177">
+        <f>H177/2+Constants!D$9-Constants!D$11</f>
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="Z177">
+        <f t="shared" si="8"/>
+        <v>83.000000000000014</v>
+      </c>
+      <c r="AA177">
+        <f t="shared" si="9"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="178" spans="1:27">
+      <c r="A178" t="s">
+        <v>230</v>
+      </c>
+      <c r="C178" t="s">
+        <v>216</v>
+      </c>
+      <c r="E178" s="41">
+        <v>2</v>
+      </c>
+      <c r="F178" t="s">
+        <v>65</v>
+      </c>
+      <c r="H178">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="I178">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="J178">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="L178">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="M178">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="N178">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="P178" t="str">
+        <f>IF(AND(J178&lt;=Constants!F$5,J178&gt;=Constants!E$5),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="Q178" t="str">
+        <f>IF(AND(J178&lt;=Constants!F$6,J178&gt;=Constants!E$6),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R178" t="str">
+        <f>IF(AND(J178&lt;=Constants!F$7,J178&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S178" t="str">
+        <f>IF(P178="N","N",IF(OR((J178+Constants!D$14)&gt;Constants!F$5,(J178-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>Y</v>
+      </c>
+      <c r="T178" t="str">
+        <f>IF(Q178="N","N",IF(OR((J178+Constants!D$14)&gt;Constants!F$6,(J178-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="U178" t="str">
+        <f>IF(R178="N","N",IF(OR((J178+Constants!D$14)&gt;Constants!F$7,(J178-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W178">
+        <f>J178/2+Constants!D$9-Constants!D$10</f>
+        <v>0.37949999999999995</v>
+      </c>
+      <c r="X178">
+        <f>H178/2+Constants!D$9-Constants!D$11</f>
+        <v>0.35749999999999993</v>
+      </c>
+      <c r="Z178">
+        <f t="shared" si="8"/>
+        <v>89.499999999999972</v>
+      </c>
+      <c r="AA178">
+        <f t="shared" si="9"/>
+        <v>67.499999999999943</v>
+      </c>
+    </row>
+    <row r="179" spans="1:27">
+      <c r="A179" t="s">
+        <v>231</v>
+      </c>
+      <c r="C179" t="s">
+        <v>217</v>
+      </c>
+      <c r="E179" s="41">
+        <v>2</v>
+      </c>
+      <c r="F179" t="s">
+        <v>65</v>
+      </c>
+      <c r="H179">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="I179">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="J179">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="L179">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="M179">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="N179">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="P179" t="str">
+        <f>IF(AND(J179&lt;=Constants!F$5,J179&gt;=Constants!E$5),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="Q179" t="str">
+        <f>IF(AND(J179&lt;=Constants!F$6,J179&gt;=Constants!E$6),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R179" t="str">
+        <f>IF(AND(J179&lt;=Constants!F$7,J179&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S179" t="str">
+        <f>IF(P179="N","N",IF(OR((J179+Constants!D$14)&gt;Constants!F$5,(J179-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>Y</v>
+      </c>
+      <c r="T179" t="str">
+        <f>IF(Q179="N","N",IF(OR((J179+Constants!D$14)&gt;Constants!F$6,(J179-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="U179" t="str">
+        <f>IF(R179="N","N",IF(OR((J179+Constants!D$14)&gt;Constants!F$7,(J179-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W179">
+        <f>J179/2+Constants!D$9-Constants!D$10</f>
+        <v>0.38</v>
+      </c>
+      <c r="X179">
+        <f>H179/2+Constants!D$9-Constants!D$11</f>
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="Z179">
+        <f t="shared" si="8"/>
+        <v>90.000000000000028</v>
+      </c>
+      <c r="AA179">
+        <f t="shared" si="9"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="180" spans="1:27">
+      <c r="A180" t="s">
+        <v>232</v>
+      </c>
+      <c r="C180" t="s">
+        <v>218</v>
+      </c>
+      <c r="E180" s="41">
+        <v>2</v>
+      </c>
+      <c r="F180" t="s">
+        <v>65</v>
+      </c>
+      <c r="H180">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="I180">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="J180">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="L180">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="M180">
+        <v>0.433</v>
+      </c>
+      <c r="N180">
+        <v>0.433</v>
+      </c>
+      <c r="P180" t="str">
+        <f>IF(AND(J180&lt;=Constants!F$5,J180&gt;=Constants!E$5),"Y","N")</f>
+        <v>N</v>
+      </c>
+      <c r="Q180" t="str">
+        <f>IF(AND(J180&lt;=Constants!F$6,J180&gt;=Constants!E$6),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="R180" t="str">
+        <f>IF(AND(J180&lt;=Constants!F$7,J180&gt;=Constants!E$7),"Y","N")</f>
+        <v>Y</v>
+      </c>
+      <c r="S180" t="str">
+        <f>IF(P180="N","N",IF(OR((J180+Constants!D$14)&gt;Constants!F$5,(J180-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
+        <v>N</v>
+      </c>
+      <c r="T180" t="str">
+        <f>IF(Q180="N","N",IF(OR((J180+Constants!D$14)&gt;Constants!F$6,(J180-Constants!D$14)&lt;Constants!E$6),"Y","Good"))</f>
+        <v>Y</v>
+      </c>
+      <c r="U180" t="str">
+        <f>IF(R180="N","N",IF(OR((J180+Constants!D$14)&gt;Constants!F$7,(J180-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
+        <v>Good</v>
+      </c>
+      <c r="W180">
+        <f>J180/2+Constants!D$9-Constants!D$10</f>
+        <v>0.37450000000000006</v>
+      </c>
+      <c r="X180">
+        <f>H180/2+Constants!D$9-Constants!D$11</f>
+        <v>0.35749999999999993</v>
+      </c>
+      <c r="Z180">
+        <f t="shared" si="8"/>
+        <v>84.500000000000071</v>
+      </c>
+      <c r="AA180">
+        <f t="shared" si="9"/>
+        <v>67.499999999999943</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="AC19:AC50">
@@ -15103,8 +16258,13 @@
     <mergeCell ref="Z17:AA17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -15114,8 +16274,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor change in plug width
</commit_message>
<xml_diff>
--- a/data/PlugWidthEvaluation.xlsx
+++ b/data/PlugWidthEvaluation.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="100" windowWidth="27800" windowHeight="14380"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1182,13 +1182,13 @@
                   <c:v>0.41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.415</c:v>
+                  <c:v>0.41499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.425</c:v>
+                  <c:v>0.42499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.43</c:v>
@@ -1200,79 +1200,79 @@
                   <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.445</c:v>
+                  <c:v>0.44500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.455</c:v>
+                  <c:v>0.45500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.465</c:v>
+                  <c:v>0.46500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.475</c:v>
+                  <c:v>0.47499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.485</c:v>
+                  <c:v>0.48499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.51</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.515</c:v>
+                  <c:v>0.51500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.525</c:v>
+                  <c:v>0.52500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.535</c:v>
+                  <c:v>0.53500000000000003</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.545</c:v>
+                  <c:v>0.54500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.555</c:v>
+                  <c:v>0.55500000000000005</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.56</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.565</c:v>
+                  <c:v>0.56499999999999995</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.57</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.575</c:v>
+                  <c:v>0.57499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.58</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.585</c:v>
+                  <c:v>0.58499999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1284,100 +1284,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>55.0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>36.0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1408,13 +1408,13 @@
                   <c:v>0.41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.415</c:v>
+                  <c:v>0.41499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.425</c:v>
+                  <c:v>0.42499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.43</c:v>
@@ -1426,79 +1426,79 @@
                   <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.445</c:v>
+                  <c:v>0.44500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.455</c:v>
+                  <c:v>0.45500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.465</c:v>
+                  <c:v>0.46500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.475</c:v>
+                  <c:v>0.47499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.485</c:v>
+                  <c:v>0.48499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.51</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.515</c:v>
+                  <c:v>0.51500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.525</c:v>
+                  <c:v>0.52500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.535</c:v>
+                  <c:v>0.53500000000000003</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.545</c:v>
+                  <c:v>0.54500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.555</c:v>
+                  <c:v>0.55500000000000005</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.56</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.565</c:v>
+                  <c:v>0.56499999999999995</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.57</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.575</c:v>
+                  <c:v>0.57499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.58</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.585</c:v>
+                  <c:v>0.58499999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1510,100 +1510,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1618,11 +1618,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2141267128"/>
-        <c:axId val="2141260280"/>
+        <c:axId val="75195904"/>
+        <c:axId val="75197824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2141267128"/>
+        <c:axId val="75195904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1651,7 +1651,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141260280"/>
+        <c:crossAx val="75197824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1659,7 +1659,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141260280"/>
+        <c:axId val="75197824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1688,7 +1688,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141267128"/>
+        <c:crossAx val="75195904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2035,19 +2035,19 @@
   <dimension ref="B2:O166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="9.1640625" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="10"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="K2" s="52"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>48</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>67.500000000000057</v>
       </c>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>0.60399999999999998</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>0.59399999999999997</v>
       </c>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="31" t="s">
         <v>165</v>
       </c>
@@ -2171,10 +2171,10 @@
         <v>0.57799999999999996</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="15" thickBot="1">
+    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>45</v>
       </c>
@@ -2195,7 +2195,7 @@
       </c>
       <c r="M9" s="35"/>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>46</v>
       </c>
@@ -2213,7 +2213,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>47</v>
       </c>
@@ -2234,7 +2234,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>152</v>
       </c>
@@ -2260,7 +2260,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2281,7 +2281,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
         <v>157</v>
       </c>
@@ -2298,7 +2298,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H15" s="36"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -2308,7 +2308,7 @@
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
     </row>
-    <row r="16" spans="2:15">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>70</v>
       </c>
@@ -2333,7 +2333,7 @@
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="17">
@@ -2356,7 +2356,7 @@
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="17">
@@ -2371,7 +2371,7 @@
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="27"/>
       <c r="D19" s="17">
@@ -2394,7 +2394,7 @@
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
     </row>
-    <row r="20" spans="2:15" ht="15" thickBot="1">
+    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4"/>
       <c r="C20" s="27"/>
       <c r="D20" s="17">
@@ -2417,7 +2417,7 @@
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
     </row>
-    <row r="21" spans="2:15">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="27"/>
       <c r="D21" s="17">
@@ -2432,7 +2432,7 @@
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
     </row>
-    <row r="22" spans="2:15">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="27"/>
       <c r="D22" s="17">
@@ -2441,7 +2441,7 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" spans="2:15">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="17">
@@ -2450,7 +2450,7 @@
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" spans="2:15">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="17">
@@ -2459,7 +2459,7 @@
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
     </row>
-    <row r="25" spans="2:15">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="17">
@@ -2468,7 +2468,7 @@
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
     </row>
-    <row r="26" spans="2:15">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="17">
@@ -2477,7 +2477,7 @@
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
     </row>
-    <row r="27" spans="2:15">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="17">
@@ -2486,7 +2486,7 @@
       <c r="N27" s="11"/>
       <c r="O27" s="11"/>
     </row>
-    <row r="28" spans="2:15">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="17">
@@ -2495,7 +2495,7 @@
       <c r="N28" s="11"/>
       <c r="O28" s="11"/>
     </row>
-    <row r="29" spans="2:15">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
       <c r="D29" s="17">
@@ -2504,7 +2504,7 @@
       <c r="N29" s="11"/>
       <c r="O29" s="11"/>
     </row>
-    <row r="30" spans="2:15">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
       <c r="D30" s="17">
@@ -2513,7 +2513,7 @@
       <c r="N30" s="11"/>
       <c r="O30" s="11"/>
     </row>
-    <row r="31" spans="2:15">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
       <c r="D31" s="17">
@@ -2522,7 +2522,7 @@
       <c r="N31" s="11"/>
       <c r="O31" s="11"/>
     </row>
-    <row r="32" spans="2:15">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
       <c r="D32" s="17">
@@ -2531,7 +2531,7 @@
       <c r="N32" s="11"/>
       <c r="O32" s="11"/>
     </row>
-    <row r="33" spans="2:15">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="17">
@@ -2540,7 +2540,7 @@
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
     </row>
-    <row r="34" spans="2:15">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
       <c r="D34" s="17">
@@ -2549,7 +2549,7 @@
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
     </row>
-    <row r="35" spans="2:15">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
       <c r="D35" s="17">
@@ -2558,681 +2558,681 @@
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
     </row>
-    <row r="36" spans="2:15">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
       <c r="D36" s="17">
         <v>0.53</v>
       </c>
     </row>
-    <row r="37" spans="2:15">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
       <c r="D37" s="17">
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="38" spans="2:15">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
       <c r="D38" s="17">
         <v>0.54</v>
       </c>
     </row>
-    <row r="39" spans="2:15">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="17">
         <v>0.54500000000000004</v>
       </c>
     </row>
-    <row r="40" spans="2:15">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
       <c r="D40" s="17">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="41" spans="2:15">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
       <c r="D41" s="17">
         <v>0.55500000000000005</v>
       </c>
     </row>
-    <row r="42" spans="2:15">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
       <c r="C42" s="5"/>
       <c r="D42" s="17">
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="43" spans="2:15">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
       <c r="C43" s="5"/>
       <c r="D43" s="17">
         <v>0.56499999999999995</v>
       </c>
     </row>
-    <row r="44" spans="2:15">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
       <c r="C44" s="5"/>
       <c r="D44" s="17">
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="45" spans="2:15">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
       <c r="C45" s="5"/>
       <c r="D45" s="17">
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="46" spans="2:15">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
       <c r="C46" s="5"/>
       <c r="D46" s="17">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="47" spans="2:15">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>
       <c r="D47" s="18">
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="48" spans="2:15">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="14"/>
     </row>
-    <row r="49" spans="2:4">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="14"/>
     </row>
-    <row r="50" spans="2:4">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="14"/>
     </row>
-    <row r="51" spans="2:4">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="14"/>
     </row>
-    <row r="52" spans="2:4">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="14"/>
     </row>
-    <row r="53" spans="2:4">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="14"/>
     </row>
-    <row r="54" spans="2:4">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="14"/>
     </row>
-    <row r="55" spans="2:4">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="14"/>
     </row>
-    <row r="56" spans="2:4">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="14"/>
     </row>
-    <row r="57" spans="2:4">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="14"/>
     </row>
-    <row r="58" spans="2:4">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="14"/>
     </row>
-    <row r="59" spans="2:4">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="14"/>
     </row>
-    <row r="60" spans="2:4">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="14"/>
     </row>
-    <row r="61" spans="2:4">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="14"/>
     </row>
-    <row r="62" spans="2:4">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="14"/>
     </row>
-    <row r="63" spans="2:4">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="14"/>
     </row>
-    <row r="64" spans="2:4">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="14"/>
     </row>
-    <row r="65" spans="2:4">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="14"/>
     </row>
-    <row r="66" spans="2:4">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="14"/>
     </row>
-    <row r="67" spans="2:4">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="14"/>
     </row>
-    <row r="68" spans="2:4">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="14"/>
     </row>
-    <row r="69" spans="2:4">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="14"/>
     </row>
-    <row r="70" spans="2:4">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="14"/>
     </row>
-    <row r="71" spans="2:4">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="14"/>
     </row>
-    <row r="72" spans="2:4">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="14"/>
     </row>
-    <row r="73" spans="2:4">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="14"/>
     </row>
-    <row r="74" spans="2:4">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="14"/>
     </row>
-    <row r="75" spans="2:4">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="14"/>
     </row>
-    <row r="76" spans="2:4">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="14"/>
     </row>
-    <row r="77" spans="2:4">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="14"/>
     </row>
-    <row r="78" spans="2:4">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="14"/>
     </row>
-    <row r="79" spans="2:4">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="14"/>
     </row>
-    <row r="80" spans="2:4">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="14"/>
     </row>
-    <row r="81" spans="2:4">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="14"/>
     </row>
-    <row r="82" spans="2:4">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="14"/>
     </row>
-    <row r="83" spans="2:4">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="14"/>
     </row>
-    <row r="84" spans="2:4">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="14"/>
     </row>
-    <row r="85" spans="2:4">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="14"/>
     </row>
-    <row r="86" spans="2:4">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="14"/>
     </row>
-    <row r="87" spans="2:4">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="14"/>
     </row>
-    <row r="88" spans="2:4">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="14"/>
     </row>
-    <row r="89" spans="2:4">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="14"/>
     </row>
-    <row r="90" spans="2:4">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="14"/>
     </row>
-    <row r="91" spans="2:4">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="28"/>
     </row>
-    <row r="92" spans="2:4">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="28"/>
     </row>
-    <row r="93" spans="2:4">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="28"/>
     </row>
-    <row r="94" spans="2:4">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="28"/>
     </row>
-    <row r="95" spans="2:4">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="28"/>
     </row>
-    <row r="96" spans="2:4">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="28"/>
     </row>
-    <row r="97" spans="2:4">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="28"/>
     </row>
-    <row r="98" spans="2:4">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="28"/>
     </row>
-    <row r="99" spans="2:4">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="28"/>
     </row>
-    <row r="100" spans="2:4">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="28"/>
     </row>
-    <row r="101" spans="2:4">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
       <c r="D101" s="28"/>
     </row>
-    <row r="102" spans="2:4">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="28"/>
     </row>
-    <row r="103" spans="2:4">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="28"/>
     </row>
-    <row r="104" spans="2:4">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="28"/>
     </row>
-    <row r="105" spans="2:4">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="28"/>
     </row>
-    <row r="106" spans="2:4">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
       <c r="D106" s="28"/>
     </row>
-    <row r="107" spans="2:4">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
       <c r="D107" s="28"/>
     </row>
-    <row r="108" spans="2:4">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
       <c r="D108" s="28"/>
     </row>
-    <row r="109" spans="2:4">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="28"/>
     </row>
-    <row r="110" spans="2:4">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="28"/>
     </row>
-    <row r="111" spans="2:4">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="28"/>
     </row>
-    <row r="112" spans="2:4">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="28"/>
     </row>
-    <row r="113" spans="2:4">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="28"/>
     </row>
-    <row r="114" spans="2:4">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
       <c r="D114" s="28"/>
     </row>
-    <row r="115" spans="2:4">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
       <c r="D115" s="28"/>
     </row>
-    <row r="116" spans="2:4">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
       <c r="D116" s="28"/>
     </row>
-    <row r="117" spans="2:4">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
       <c r="D117" s="28"/>
     </row>
-    <row r="118" spans="2:4">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
       <c r="D118" s="28"/>
     </row>
-    <row r="119" spans="2:4">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
       <c r="D119" s="28"/>
     </row>
-    <row r="120" spans="2:4">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
       <c r="D120" s="28"/>
     </row>
-    <row r="121" spans="2:4">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
       <c r="D121" s="28"/>
     </row>
-    <row r="122" spans="2:4">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
       <c r="D122" s="28"/>
     </row>
-    <row r="123" spans="2:4">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="5"/>
       <c r="C123" s="5"/>
       <c r="D123" s="28"/>
     </row>
-    <row r="124" spans="2:4">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
       <c r="D124" s="28"/>
     </row>
-    <row r="125" spans="2:4">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
       <c r="D125" s="28"/>
     </row>
-    <row r="126" spans="2:4">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
       <c r="D126" s="28"/>
     </row>
-    <row r="127" spans="2:4">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
       <c r="D127" s="28"/>
     </row>
-    <row r="128" spans="2:4">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
       <c r="D128" s="28"/>
     </row>
-    <row r="129" spans="2:4">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
       <c r="D129" s="28"/>
     </row>
-    <row r="130" spans="2:4">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
       <c r="D130" s="28"/>
     </row>
-    <row r="131" spans="2:4">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
       <c r="D131" s="28"/>
     </row>
-    <row r="132" spans="2:4">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
       <c r="D132" s="28"/>
     </row>
-    <row r="133" spans="2:4">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
       <c r="D133" s="28"/>
     </row>
-    <row r="134" spans="2:4">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
       <c r="D134" s="28"/>
     </row>
-    <row r="135" spans="2:4">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
       <c r="D135" s="28"/>
     </row>
-    <row r="136" spans="2:4">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
       <c r="D136" s="28"/>
     </row>
-    <row r="137" spans="2:4">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
       <c r="D137" s="28"/>
     </row>
-    <row r="138" spans="2:4">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
       <c r="D138" s="28"/>
     </row>
-    <row r="139" spans="2:4">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
       <c r="D139" s="28"/>
     </row>
-    <row r="140" spans="2:4">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
       <c r="D140" s="28"/>
     </row>
-    <row r="141" spans="2:4">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
       <c r="D141" s="28"/>
     </row>
-    <row r="142" spans="2:4">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
       <c r="D142" s="28"/>
     </row>
-    <row r="143" spans="2:4">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
       <c r="D143" s="28"/>
     </row>
-    <row r="144" spans="2:4">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
       <c r="D144" s="28"/>
     </row>
-    <row r="145" spans="2:4">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
       <c r="D145" s="28"/>
     </row>
-    <row r="146" spans="2:4">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
       <c r="D146" s="28"/>
     </row>
-    <row r="147" spans="2:4">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
       <c r="D147" s="28"/>
     </row>
-    <row r="148" spans="2:4">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" s="5"/>
       <c r="C148" s="5"/>
       <c r="D148" s="28"/>
     </row>
-    <row r="149" spans="2:4">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
       <c r="D149" s="28"/>
     </row>
-    <row r="150" spans="2:4">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
       <c r="D150" s="28"/>
     </row>
-    <row r="151" spans="2:4">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
       <c r="D151" s="28"/>
     </row>
-    <row r="152" spans="2:4">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
       <c r="D152" s="28"/>
     </row>
-    <row r="153" spans="2:4">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
       <c r="D153" s="28"/>
     </row>
-    <row r="154" spans="2:4">
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B154" s="5"/>
       <c r="C154" s="5"/>
       <c r="D154" s="28"/>
     </row>
-    <row r="155" spans="2:4">
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
       <c r="D155" s="28"/>
     </row>
-    <row r="156" spans="2:4">
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B156" s="5"/>
       <c r="C156" s="5"/>
       <c r="D156" s="28"/>
     </row>
-    <row r="157" spans="2:4">
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B157" s="5"/>
       <c r="C157" s="5"/>
       <c r="D157" s="28"/>
     </row>
-    <row r="158" spans="2:4">
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
       <c r="D158" s="28"/>
     </row>
-    <row r="159" spans="2:4">
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
       <c r="D159" s="28"/>
     </row>
-    <row r="160" spans="2:4">
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
       <c r="D160" s="28"/>
     </row>
-    <row r="161" spans="2:4">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
       <c r="D161" s="28"/>
     </row>
-    <row r="162" spans="2:4">
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="5"/>
       <c r="C162" s="5"/>
       <c r="D162" s="28"/>
     </row>
-    <row r="163" spans="2:4">
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
       <c r="D163" s="28"/>
     </row>
-    <row r="164" spans="2:4">
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
       <c r="D164" s="28"/>
     </row>
-    <row r="165" spans="2:4">
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
       <c r="D165" s="28"/>
     </row>
-    <row r="166" spans="2:4">
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="5"/>
       <c r="C166" s="5"/>
       <c r="D166" s="28"/>
@@ -3259,31 +3259,31 @@
     <sheetView workbookViewId="0">
       <pane ySplit="16" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="AC178" sqref="AC178"/>
+      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="1.5" customWidth="1"/>
-    <col min="5" max="6" width="7.6640625" customWidth="1"/>
-    <col min="7" max="7" width="1.5" customWidth="1"/>
-    <col min="8" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="1.5" customWidth="1"/>
-    <col min="12" max="14" width="9.6640625" customWidth="1"/>
-    <col min="15" max="15" width="1.5" customWidth="1"/>
-    <col min="16" max="21" width="8.6640625" customWidth="1"/>
-    <col min="22" max="22" width="1.5" customWidth="1"/>
-    <col min="23" max="24" width="10.6640625" customWidth="1"/>
-    <col min="25" max="25" width="1.5" customWidth="1"/>
-    <col min="26" max="27" width="10.6640625" customWidth="1"/>
-    <col min="28" max="28" width="1.5" customWidth="1"/>
-    <col min="31" max="31" width="1.5" customWidth="1"/>
-    <col min="37" max="37" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="1.42578125" customWidth="1"/>
+    <col min="5" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="1.42578125" customWidth="1"/>
+    <col min="8" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="1.42578125" customWidth="1"/>
+    <col min="12" max="14" width="9.7109375" customWidth="1"/>
+    <col min="15" max="15" width="1.42578125" customWidth="1"/>
+    <col min="16" max="21" width="8.7109375" customWidth="1"/>
+    <col min="22" max="22" width="1.42578125" customWidth="1"/>
+    <col min="23" max="24" width="10.7109375" customWidth="1"/>
+    <col min="25" max="25" width="1.42578125" customWidth="1"/>
+    <col min="26" max="27" width="10.7109375" customWidth="1"/>
+    <col min="28" max="28" width="1.42578125" customWidth="1"/>
+    <col min="31" max="31" width="1.42578125" customWidth="1"/>
+    <col min="37" max="37" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="17" spans="1:39" ht="15" thickBot="1">
+    <row r="17" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="AM17" s="57"/>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>52</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:39">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:39">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:39">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:39">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -4201,7 +4201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:39">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:39">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:39">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:39">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:39">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -4796,7 +4796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:39">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>56</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:39">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:39">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:39">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -5391,7 +5391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:39">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:39">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -5561,7 +5561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:39">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:39">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:39">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -5816,7 +5816,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:39">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:39">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -5986,7 +5986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:39">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:39">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -6155,7 +6155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:39" ht="15" thickBot="1">
+    <row r="51" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:39" ht="15" thickBot="1">
+    <row r="52" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:39">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -6371,7 +6371,7 @@
       <c r="AF53" s="24"/>
       <c r="AG53" s="11"/>
     </row>
-    <row r="54" spans="1:39">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -6450,7 +6450,7 @@
       <c r="AF54" s="24"/>
       <c r="AG54" s="11"/>
     </row>
-    <row r="55" spans="1:39">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -6529,7 +6529,7 @@
       <c r="AF55" s="24"/>
       <c r="AG55" s="11"/>
     </row>
-    <row r="56" spans="1:39">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -6608,7 +6608,7 @@
       <c r="AF56" s="24"/>
       <c r="AG56" s="11"/>
     </row>
-    <row r="57" spans="1:39">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -6687,7 +6687,7 @@
       <c r="AF57" s="24"/>
       <c r="AG57" s="11"/>
     </row>
-    <row r="58" spans="1:39">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -6766,7 +6766,7 @@
       <c r="AF58" s="24"/>
       <c r="AG58" s="11"/>
     </row>
-    <row r="59" spans="1:39">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -6845,7 +6845,7 @@
       <c r="AF59" s="24"/>
       <c r="AG59" s="11"/>
     </row>
-    <row r="60" spans="1:39">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -6924,7 +6924,7 @@
       <c r="AF60" s="24"/>
       <c r="AG60" s="11"/>
     </row>
-    <row r="61" spans="1:39">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -7003,7 +7003,7 @@
       <c r="AF61" s="24"/>
       <c r="AG61" s="11"/>
     </row>
-    <row r="62" spans="1:39">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -7082,7 +7082,7 @@
       <c r="AF62" s="24"/>
       <c r="AG62" s="11"/>
     </row>
-    <row r="63" spans="1:39">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -7161,7 +7161,7 @@
       <c r="AF63" s="24"/>
       <c r="AG63" s="11"/>
     </row>
-    <row r="64" spans="1:39">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>59</v>
       </c>
@@ -7240,7 +7240,7 @@
       <c r="AF64" s="24"/>
       <c r="AG64" s="11"/>
     </row>
-    <row r="65" spans="1:33">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>59</v>
       </c>
@@ -7319,7 +7319,7 @@
       <c r="AF65" s="24"/>
       <c r="AG65" s="11"/>
     </row>
-    <row r="66" spans="1:33">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>59</v>
       </c>
@@ -7398,7 +7398,7 @@
       <c r="AF66" s="24"/>
       <c r="AG66" s="11"/>
     </row>
-    <row r="67" spans="1:33">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>59</v>
       </c>
@@ -7477,7 +7477,7 @@
       <c r="AF67" s="24"/>
       <c r="AG67" s="11"/>
     </row>
-    <row r="68" spans="1:33">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>59</v>
       </c>
@@ -7556,7 +7556,7 @@
       <c r="AF68" s="24"/>
       <c r="AG68" s="11"/>
     </row>
-    <row r="69" spans="1:33">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>59</v>
       </c>
@@ -7635,7 +7635,7 @@
       <c r="AF69" s="24"/>
       <c r="AG69" s="11"/>
     </row>
-    <row r="70" spans="1:33">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>59</v>
       </c>
@@ -7714,7 +7714,7 @@
       <c r="AF70" s="24"/>
       <c r="AG70" s="11"/>
     </row>
-    <row r="71" spans="1:33">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>59</v>
       </c>
@@ -7793,7 +7793,7 @@
       <c r="AF71" s="24"/>
       <c r="AG71" s="11"/>
     </row>
-    <row r="72" spans="1:33">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>59</v>
       </c>
@@ -7872,7 +7872,7 @@
       <c r="AF72" s="24"/>
       <c r="AG72" s="11"/>
     </row>
-    <row r="73" spans="1:33">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>59</v>
       </c>
@@ -7951,7 +7951,7 @@
       <c r="AF73" s="24"/>
       <c r="AG73" s="11"/>
     </row>
-    <row r="74" spans="1:33">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>59</v>
       </c>
@@ -8030,7 +8030,7 @@
       <c r="AF74" s="24"/>
       <c r="AG74" s="11"/>
     </row>
-    <row r="75" spans="1:33">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>59</v>
       </c>
@@ -8109,7 +8109,7 @@
       <c r="AF75" s="24"/>
       <c r="AG75" s="11"/>
     </row>
-    <row r="76" spans="1:33">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>59</v>
       </c>
@@ -8188,7 +8188,7 @@
       <c r="AF76" s="24"/>
       <c r="AG76" s="11"/>
     </row>
-    <row r="77" spans="1:33">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>59</v>
       </c>
@@ -8267,7 +8267,7 @@
       <c r="AF77" s="24"/>
       <c r="AG77" s="11"/>
     </row>
-    <row r="78" spans="1:33">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>59</v>
       </c>
@@ -8346,7 +8346,7 @@
       <c r="AF78" s="24"/>
       <c r="AG78" s="11"/>
     </row>
-    <row r="79" spans="1:33">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>59</v>
       </c>
@@ -8425,7 +8425,7 @@
       <c r="AF79" s="24"/>
       <c r="AG79" s="11"/>
     </row>
-    <row r="80" spans="1:33">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>59</v>
       </c>
@@ -8504,7 +8504,7 @@
       <c r="AF80" s="24"/>
       <c r="AG80" s="11"/>
     </row>
-    <row r="81" spans="1:33">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>59</v>
       </c>
@@ -8583,7 +8583,7 @@
       <c r="AF81" s="24"/>
       <c r="AG81" s="11"/>
     </row>
-    <row r="82" spans="1:33">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>59</v>
       </c>
@@ -8662,7 +8662,7 @@
       <c r="AF82" s="24"/>
       <c r="AG82" s="11"/>
     </row>
-    <row r="83" spans="1:33">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>59</v>
       </c>
@@ -8741,7 +8741,7 @@
       <c r="AF83" s="24"/>
       <c r="AG83" s="11"/>
     </row>
-    <row r="84" spans="1:33">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>59</v>
       </c>
@@ -8820,7 +8820,7 @@
       <c r="AF84" s="24"/>
       <c r="AG84" s="11"/>
     </row>
-    <row r="85" spans="1:33">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>59</v>
       </c>
@@ -8899,7 +8899,7 @@
       <c r="AF85" s="24"/>
       <c r="AG85" s="11"/>
     </row>
-    <row r="86" spans="1:33">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>59</v>
       </c>
@@ -8978,7 +8978,7 @@
       <c r="AF86" s="24"/>
       <c r="AG86" s="11"/>
     </row>
-    <row r="87" spans="1:33">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>59</v>
       </c>
@@ -9057,7 +9057,7 @@
       <c r="AF87" s="24"/>
       <c r="AG87" s="11"/>
     </row>
-    <row r="88" spans="1:33">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>59</v>
       </c>
@@ -9136,7 +9136,7 @@
       <c r="AF88" s="24"/>
       <c r="AG88" s="11"/>
     </row>
-    <row r="89" spans="1:33">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>59</v>
       </c>
@@ -9215,7 +9215,7 @@
       <c r="AF89" s="24"/>
       <c r="AG89" s="11"/>
     </row>
-    <row r="90" spans="1:33">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>59</v>
       </c>
@@ -9294,7 +9294,7 @@
       <c r="AF90" s="24"/>
       <c r="AG90" s="11"/>
     </row>
-    <row r="91" spans="1:33">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>59</v>
       </c>
@@ -9373,7 +9373,7 @@
       <c r="AF91" s="24"/>
       <c r="AG91" s="11"/>
     </row>
-    <row r="92" spans="1:33">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>59</v>
       </c>
@@ -9452,7 +9452,7 @@
       <c r="AF92" s="24"/>
       <c r="AG92" s="11"/>
     </row>
-    <row r="93" spans="1:33">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>59</v>
       </c>
@@ -9531,7 +9531,7 @@
       <c r="AF93" s="24"/>
       <c r="AG93" s="11"/>
     </row>
-    <row r="94" spans="1:33">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>59</v>
       </c>
@@ -9610,7 +9610,7 @@
       <c r="AF94" s="24"/>
       <c r="AG94" s="11"/>
     </row>
-    <row r="95" spans="1:33">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>59</v>
       </c>
@@ -9689,7 +9689,7 @@
       <c r="AF95" s="24"/>
       <c r="AG95" s="11"/>
     </row>
-    <row r="96" spans="1:33">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>59</v>
       </c>
@@ -9768,7 +9768,7 @@
       <c r="AF96" s="24"/>
       <c r="AG96" s="11"/>
     </row>
-    <row r="97" spans="1:33">
+    <row r="97" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>59</v>
       </c>
@@ -9847,7 +9847,7 @@
       <c r="AF97" s="24"/>
       <c r="AG97" s="11"/>
     </row>
-    <row r="98" spans="1:33">
+    <row r="98" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>59</v>
       </c>
@@ -9917,7 +9917,7 @@
       <c r="AF98" s="24"/>
       <c r="AG98" s="11"/>
     </row>
-    <row r="99" spans="1:33">
+    <row r="99" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>59</v>
       </c>
@@ -9996,7 +9996,7 @@
       <c r="AF99" s="24"/>
       <c r="AG99" s="11"/>
     </row>
-    <row r="100" spans="1:33">
+    <row r="100" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>59</v>
       </c>
@@ -10075,7 +10075,7 @@
       <c r="AF100" s="24"/>
       <c r="AG100" s="11"/>
     </row>
-    <row r="101" spans="1:33">
+    <row r="101" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>59</v>
       </c>
@@ -10154,7 +10154,7 @@
       <c r="AF101" s="24"/>
       <c r="AG101" s="11"/>
     </row>
-    <row r="102" spans="1:33">
+    <row r="102" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>59</v>
       </c>
@@ -10233,7 +10233,7 @@
       <c r="AF102" s="24"/>
       <c r="AG102" s="11"/>
     </row>
-    <row r="103" spans="1:33">
+    <row r="103" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>59</v>
       </c>
@@ -10312,7 +10312,7 @@
       <c r="AF103" s="24"/>
       <c r="AG103" s="11"/>
     </row>
-    <row r="104" spans="1:33">
+    <row r="104" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>59</v>
       </c>
@@ -10391,7 +10391,7 @@
       <c r="AF104" s="24"/>
       <c r="AG104" s="11"/>
     </row>
-    <row r="105" spans="1:33">
+    <row r="105" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>59</v>
       </c>
@@ -10470,7 +10470,7 @@
       <c r="AF105" s="24"/>
       <c r="AG105" s="11"/>
     </row>
-    <row r="106" spans="1:33">
+    <row r="106" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>59</v>
       </c>
@@ -10549,7 +10549,7 @@
       <c r="AF106" s="24"/>
       <c r="AG106" s="11"/>
     </row>
-    <row r="107" spans="1:33">
+    <row r="107" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>59</v>
       </c>
@@ -10628,7 +10628,7 @@
       <c r="AF107" s="24"/>
       <c r="AG107" s="11"/>
     </row>
-    <row r="108" spans="1:33">
+    <row r="108" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>59</v>
       </c>
@@ -10707,7 +10707,7 @@
       <c r="AF108" s="24"/>
       <c r="AG108" s="11"/>
     </row>
-    <row r="109" spans="1:33">
+    <row r="109" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>59</v>
       </c>
@@ -10786,7 +10786,7 @@
       <c r="AF109" s="24"/>
       <c r="AG109" s="11"/>
     </row>
-    <row r="110" spans="1:33">
+    <row r="110" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>59</v>
       </c>
@@ -10865,7 +10865,7 @@
       <c r="AF110" s="24"/>
       <c r="AG110" s="11"/>
     </row>
-    <row r="111" spans="1:33">
+    <row r="111" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>59</v>
       </c>
@@ -10944,7 +10944,7 @@
       <c r="AF111" s="24"/>
       <c r="AG111" s="11"/>
     </row>
-    <row r="112" spans="1:33">
+    <row r="112" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>59</v>
       </c>
@@ -11023,7 +11023,7 @@
       <c r="AF112" s="24"/>
       <c r="AG112" s="11"/>
     </row>
-    <row r="113" spans="1:33">
+    <row r="113" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>59</v>
       </c>
@@ -11102,7 +11102,7 @@
       <c r="AF113" s="24"/>
       <c r="AG113" s="11"/>
     </row>
-    <row r="114" spans="1:33">
+    <row r="114" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>59</v>
       </c>
@@ -11181,7 +11181,7 @@
       <c r="AF114" s="24"/>
       <c r="AG114" s="11"/>
     </row>
-    <row r="115" spans="1:33">
+    <row r="115" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>59</v>
       </c>
@@ -11260,7 +11260,7 @@
       <c r="AF115" s="24"/>
       <c r="AG115" s="11"/>
     </row>
-    <row r="116" spans="1:33">
+    <row r="116" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>59</v>
       </c>
@@ -11339,7 +11339,7 @@
       <c r="AF116" s="24"/>
       <c r="AG116" s="11"/>
     </row>
-    <row r="117" spans="1:33">
+    <row r="117" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>59</v>
       </c>
@@ -11418,7 +11418,7 @@
       <c r="AF117" s="24"/>
       <c r="AG117" s="11"/>
     </row>
-    <row r="118" spans="1:33">
+    <row r="118" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>59</v>
       </c>
@@ -11497,7 +11497,7 @@
       <c r="AF118" s="24"/>
       <c r="AG118" s="11"/>
     </row>
-    <row r="119" spans="1:33">
+    <row r="119" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>59</v>
       </c>
@@ -11576,7 +11576,7 @@
       <c r="AF119" s="24"/>
       <c r="AG119" s="11"/>
     </row>
-    <row r="120" spans="1:33">
+    <row r="120" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>59</v>
       </c>
@@ -11655,7 +11655,7 @@
       <c r="AF120" s="24"/>
       <c r="AG120" s="11"/>
     </row>
-    <row r="121" spans="1:33">
+    <row r="121" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>59</v>
       </c>
@@ -11734,7 +11734,7 @@
       <c r="AF121" s="24"/>
       <c r="AG121" s="11"/>
     </row>
-    <row r="122" spans="1:33">
+    <row r="122" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>59</v>
       </c>
@@ -11813,7 +11813,7 @@
       <c r="AF122" s="24"/>
       <c r="AG122" s="11"/>
     </row>
-    <row r="123" spans="1:33">
+    <row r="123" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>59</v>
       </c>
@@ -11892,7 +11892,7 @@
       <c r="AF123" s="24"/>
       <c r="AG123" s="11"/>
     </row>
-    <row r="124" spans="1:33">
+    <row r="124" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>59</v>
       </c>
@@ -11971,7 +11971,7 @@
       <c r="AF124" s="24"/>
       <c r="AG124" s="11"/>
     </row>
-    <row r="125" spans="1:33">
+    <row r="125" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>59</v>
       </c>
@@ -12050,7 +12050,7 @@
       <c r="AF125" s="24"/>
       <c r="AG125" s="11"/>
     </row>
-    <row r="126" spans="1:33">
+    <row r="126" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>59</v>
       </c>
@@ -12129,7 +12129,7 @@
       <c r="AF126" s="24"/>
       <c r="AG126" s="11"/>
     </row>
-    <row r="127" spans="1:33">
+    <row r="127" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>59</v>
       </c>
@@ -12208,7 +12208,7 @@
       <c r="AF127" s="24"/>
       <c r="AG127" s="11"/>
     </row>
-    <row r="128" spans="1:33">
+    <row r="128" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>59</v>
       </c>
@@ -12287,7 +12287,7 @@
       <c r="AF128" s="24"/>
       <c r="AG128" s="11"/>
     </row>
-    <row r="129" spans="1:33">
+    <row r="129" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>59</v>
       </c>
@@ -12366,7 +12366,7 @@
       <c r="AF129" s="24"/>
       <c r="AG129" s="11"/>
     </row>
-    <row r="130" spans="1:33">
+    <row r="130" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>59</v>
       </c>
@@ -12445,7 +12445,7 @@
       <c r="AF130" s="24"/>
       <c r="AG130" s="11"/>
     </row>
-    <row r="131" spans="1:33">
+    <row r="131" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>59</v>
       </c>
@@ -12524,7 +12524,7 @@
       <c r="AF131" s="24"/>
       <c r="AG131" s="11"/>
     </row>
-    <row r="132" spans="1:33">
+    <row r="132" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>170</v>
       </c>
@@ -12594,7 +12594,7 @@
       <c r="AF132" s="24"/>
       <c r="AG132" s="11"/>
     </row>
-    <row r="133" spans="1:33">
+    <row r="133" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>170</v>
       </c>
@@ -12664,7 +12664,7 @@
       <c r="AF133" s="24"/>
       <c r="AG133" s="11"/>
     </row>
-    <row r="134" spans="1:33">
+    <row r="134" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>173</v>
       </c>
@@ -12740,7 +12740,7 @@
       <c r="AF134" s="24"/>
       <c r="AG134" s="11"/>
     </row>
-    <row r="135" spans="1:33">
+    <row r="135" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>173</v>
       </c>
@@ -12816,7 +12816,7 @@
       <c r="AF135" s="24"/>
       <c r="AG135" s="11"/>
     </row>
-    <row r="136" spans="1:33">
+    <row r="136" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>173</v>
       </c>
@@ -12892,7 +12892,7 @@
       <c r="AF136" s="24"/>
       <c r="AG136" s="11"/>
     </row>
-    <row r="137" spans="1:33">
+    <row r="137" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>173</v>
       </c>
@@ -12968,7 +12968,7 @@
       <c r="AF137" s="24"/>
       <c r="AG137" s="11"/>
     </row>
-    <row r="138" spans="1:33">
+    <row r="138" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>173</v>
       </c>
@@ -13044,7 +13044,7 @@
       <c r="AF138" s="24"/>
       <c r="AG138" s="11"/>
     </row>
-    <row r="139" spans="1:33">
+    <row r="139" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>173</v>
       </c>
@@ -13120,7 +13120,7 @@
       <c r="AF139" s="24"/>
       <c r="AG139" s="11"/>
     </row>
-    <row r="140" spans="1:33">
+    <row r="140" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>173</v>
       </c>
@@ -13196,7 +13196,7 @@
       <c r="AF140" s="24"/>
       <c r="AG140" s="11"/>
     </row>
-    <row r="141" spans="1:33">
+    <row r="141" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>173</v>
       </c>
@@ -13272,7 +13272,7 @@
       <c r="AF141" s="24"/>
       <c r="AG141" s="11"/>
     </row>
-    <row r="142" spans="1:33">
+    <row r="142" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>173</v>
       </c>
@@ -13348,7 +13348,7 @@
       <c r="AF142" s="24"/>
       <c r="AG142" s="11"/>
     </row>
-    <row r="143" spans="1:33">
+    <row r="143" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>173</v>
       </c>
@@ -13424,7 +13424,7 @@
       <c r="AF143" s="24"/>
       <c r="AG143" s="11"/>
     </row>
-    <row r="144" spans="1:33">
+    <row r="144" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>173</v>
       </c>
@@ -13500,7 +13500,7 @@
       <c r="AF144" s="24"/>
       <c r="AG144" s="11"/>
     </row>
-    <row r="145" spans="1:33">
+    <row r="145" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>173</v>
       </c>
@@ -13576,7 +13576,7 @@
       <c r="AF145" s="24"/>
       <c r="AG145" s="11"/>
     </row>
-    <row r="146" spans="1:33">
+    <row r="146" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>173</v>
       </c>
@@ -13652,7 +13652,7 @@
       <c r="AF146" s="24"/>
       <c r="AG146" s="11"/>
     </row>
-    <row r="147" spans="1:33">
+    <row r="147" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>173</v>
       </c>
@@ -13728,7 +13728,7 @@
       <c r="AF147" s="24"/>
       <c r="AG147" s="11"/>
     </row>
-    <row r="148" spans="1:33">
+    <row r="148" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>173</v>
       </c>
@@ -13804,7 +13804,7 @@
       <c r="AF148" s="24"/>
       <c r="AG148" s="11"/>
     </row>
-    <row r="149" spans="1:33">
+    <row r="149" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>173</v>
       </c>
@@ -13880,7 +13880,7 @@
       <c r="AF149" s="24"/>
       <c r="AG149" s="11"/>
     </row>
-    <row r="150" spans="1:33">
+    <row r="150" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>173</v>
       </c>
@@ -13956,7 +13956,7 @@
       <c r="AF150" s="24"/>
       <c r="AG150" s="11"/>
     </row>
-    <row r="151" spans="1:33">
+    <row r="151" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>173</v>
       </c>
@@ -14032,7 +14032,7 @@
       <c r="AF151" s="24"/>
       <c r="AG151" s="11"/>
     </row>
-    <row r="152" spans="1:33">
+    <row r="152" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>173</v>
       </c>
@@ -14108,7 +14108,7 @@
       <c r="AF152" s="24"/>
       <c r="AG152" s="11"/>
     </row>
-    <row r="153" spans="1:33">
+    <row r="153" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>173</v>
       </c>
@@ -14184,7 +14184,7 @@
       <c r="AF153" s="24"/>
       <c r="AG153" s="11"/>
     </row>
-    <row r="154" spans="1:33">
+    <row r="154" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>173</v>
       </c>
@@ -14260,7 +14260,7 @@
       <c r="AF154" s="24"/>
       <c r="AG154" s="11"/>
     </row>
-    <row r="155" spans="1:33">
+    <row r="155" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>173</v>
       </c>
@@ -14336,7 +14336,7 @@
       <c r="AF155" s="24"/>
       <c r="AG155" s="11"/>
     </row>
-    <row r="156" spans="1:33">
+    <row r="156" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>173</v>
       </c>
@@ -14412,7 +14412,7 @@
       <c r="AF156" s="24"/>
       <c r="AG156" s="11"/>
     </row>
-    <row r="157" spans="1:33">
+    <row r="157" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>173</v>
       </c>
@@ -14488,7 +14488,7 @@
       <c r="AF157" s="24"/>
       <c r="AG157" s="11"/>
     </row>
-    <row r="158" spans="1:33">
+    <row r="158" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>173</v>
       </c>
@@ -14564,7 +14564,7 @@
       <c r="AF158" s="24"/>
       <c r="AG158" s="11"/>
     </row>
-    <row r="159" spans="1:33">
+    <row r="159" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>173</v>
       </c>
@@ -14640,7 +14640,7 @@
       <c r="AF159" s="24"/>
       <c r="AG159" s="11"/>
     </row>
-    <row r="160" spans="1:33">
+    <row r="160" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>173</v>
       </c>
@@ -14716,7 +14716,7 @@
       <c r="AF160" s="24"/>
       <c r="AG160" s="11"/>
     </row>
-    <row r="161" spans="1:35">
+    <row r="161" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>173</v>
       </c>
@@ -14792,7 +14792,7 @@
       <c r="AF161" s="24"/>
       <c r="AG161" s="11"/>
     </row>
-    <row r="162" spans="1:35">
+    <row r="162" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>173</v>
       </c>
@@ -14868,7 +14868,7 @@
       <c r="AF162" s="24"/>
       <c r="AG162" s="11"/>
     </row>
-    <row r="163" spans="1:35">
+    <row r="163" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>173</v>
       </c>
@@ -14944,7 +14944,7 @@
       <c r="AF163" s="24"/>
       <c r="AG163" s="11"/>
     </row>
-    <row r="164" spans="1:35">
+    <row r="164" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>173</v>
       </c>
@@ -15020,7 +15020,7 @@
       <c r="AF164" s="24"/>
       <c r="AG164" s="11"/>
     </row>
-    <row r="165" spans="1:35">
+    <row r="165" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>173</v>
       </c>
@@ -15096,7 +15096,7 @@
       <c r="AF165" s="24"/>
       <c r="AG165" s="11"/>
     </row>
-    <row r="166" spans="1:35">
+    <row r="166" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>204</v>
       </c>
@@ -15172,7 +15172,7 @@
       <c r="AF166" s="24"/>
       <c r="AG166" s="11"/>
     </row>
-    <row r="167" spans="1:35">
+    <row r="167" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>219</v>
       </c>
@@ -15248,7 +15248,7 @@
       <c r="AF167" s="24"/>
       <c r="AG167" s="11"/>
     </row>
-    <row r="168" spans="1:35">
+    <row r="168" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>220</v>
       </c>
@@ -15324,7 +15324,7 @@
       <c r="AF168" s="24"/>
       <c r="AG168" s="11"/>
     </row>
-    <row r="169" spans="1:35">
+    <row r="169" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>221</v>
       </c>
@@ -15403,7 +15403,7 @@
       <c r="AH169" s="5"/>
       <c r="AI169" s="5"/>
     </row>
-    <row r="170" spans="1:35">
+    <row r="170" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>222</v>
       </c>
@@ -15482,7 +15482,7 @@
       <c r="AH170" s="5"/>
       <c r="AI170" s="5"/>
     </row>
-    <row r="171" spans="1:35">
+    <row r="171" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>223</v>
       </c>
@@ -15561,7 +15561,7 @@
       <c r="AH171" s="5"/>
       <c r="AI171" s="5"/>
     </row>
-    <row r="172" spans="1:35">
+    <row r="172" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>224</v>
       </c>
@@ -15640,7 +15640,7 @@
       <c r="AH172" s="5"/>
       <c r="AI172" s="5"/>
     </row>
-    <row r="173" spans="1:35">
+    <row r="173" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>225</v>
       </c>
@@ -15719,7 +15719,7 @@
       <c r="AH173" s="5"/>
       <c r="AI173" s="5"/>
     </row>
-    <row r="174" spans="1:35">
+    <row r="174" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>226</v>
       </c>
@@ -15798,7 +15798,7 @@
       <c r="AH174" s="5"/>
       <c r="AI174" s="5"/>
     </row>
-    <row r="175" spans="1:35">
+    <row r="175" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>227</v>
       </c>
@@ -15877,7 +15877,7 @@
       <c r="AH175" s="5"/>
       <c r="AI175" s="5"/>
     </row>
-    <row r="176" spans="1:35">
+    <row r="176" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>228</v>
       </c>
@@ -15953,7 +15953,7 @@
       <c r="AF176" s="5"/>
       <c r="AG176" s="5"/>
     </row>
-    <row r="177" spans="1:27">
+    <row r="177" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>229</v>
       </c>
@@ -16025,7 +16025,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="178" spans="1:27">
+    <row r="178" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>230</v>
       </c>
@@ -16097,7 +16097,7 @@
         <v>67.499999999999943</v>
       </c>
     </row>
-    <row r="179" spans="1:27">
+    <row r="179" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>231</v>
       </c>
@@ -16169,7 +16169,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="180" spans="1:27">
+    <row r="180" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>232</v>
       </c>
@@ -16274,7 +16274,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
changed v5 of AC3 to be .366
</commit_message>
<xml_diff>
--- a/data/PlugWidthEvaluation.xlsx
+++ b/data/PlugWidthEvaluation.xlsx
@@ -1147,7 +1147,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1618,11 +1617,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="75195904"/>
-        <c:axId val="75197824"/>
+        <c:axId val="138041216"/>
+        <c:axId val="138055680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75195904"/>
+        <c:axId val="138041216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1644,14 +1643,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75197824"/>
+        <c:crossAx val="138055680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1659,7 +1657,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75197824"/>
+        <c:axId val="138055680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1681,21 +1679,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75195904"/>
+        <c:crossAx val="138041216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2035,7 +2031,7 @@
   <dimension ref="B2:O166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,19 +2152,19 @@
         <v>165</v>
       </c>
       <c r="C7" s="32">
-        <v>0.36499999999999999</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="D7" s="15">
         <f>C7-0.29</f>
-        <v>7.5000000000000011E-2</v>
+        <v>7.6000000000000012E-2</v>
       </c>
       <c r="E7" s="8">
         <f t="shared" si="0"/>
-        <v>0.53400000000000003</v>
+        <v>0.53600000000000003</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" si="1"/>
-        <v>0.57799999999999996</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2385,11 +2381,11 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5">
         <f>COUNTIF(Data!R19:R1000,"Y")</f>
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M19" s="37">
         <f>COUNTIF(Data!R19:R1000,"N")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
@@ -2408,11 +2404,11 @@
       <c r="K20" s="39"/>
       <c r="L20" s="39">
         <f>COUNTIF(Data!U19:U1000,"Good")</f>
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M20" s="40">
         <f>L9-L20</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
@@ -12705,7 +12701,7 @@
       </c>
       <c r="R134" t="str">
         <f>IF(AND(J134&lt;=Constants!F$7,J134&gt;=Constants!E$7),"Y","N")</f>
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="S134" t="str">
         <f>IF(P134="N","N",IF(OR((J134+Constants!D$14)&gt;Constants!F$5,(J134-Constants!D$14)&lt;Constants!E$5),"Y","Good"))</f>
@@ -12717,7 +12713,7 @@
       </c>
       <c r="U134" t="str">
         <f>IF(R134="N","N",IF(OR((J134+Constants!D$14)&gt;Constants!F$7,(J134-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="W134">
         <f>J134/2+Constants!D$9-Constants!D$10</f>
@@ -14617,7 +14613,7 @@
       </c>
       <c r="U159" t="str">
         <f>IF(R159="N","N",IF(OR((J159+Constants!D$14)&gt;Constants!F$7,(J159-Constants!D$14)&lt;Constants!E$7),"Y","Good"))</f>
-        <v>Good</v>
+        <v>Y</v>
       </c>
       <c r="W159">
         <f>J159/2+Constants!D$9-Constants!D$10</f>

</xml_diff>